<commit_message>
Calculate CV of actual and normals for each site, write to CSV; and write percent deviation from normals to csv
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.3_months-to-include-for-precip-normals-comparison.xlsx
+++ b/data/data-wrangling-intermediate/03.3_months-to-include-for-precip-normals-comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3392" documentId="8_{89B2EEDE-D508-4F25-B24C-4C204CBA613B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15921AE2-CB65-4F9F-8ECA-8119B0F34594}"/>
+  <xr:revisionPtr revIDLastSave="3393" documentId="8_{89B2EEDE-D508-4F25-B24C-4C204CBA613B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{600068E6-2B54-4047-80A6-DEAB794755CF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{1028A4EE-DCCB-47E3-9760-4B4BA3E1195B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{1028A4EE-DCCB-47E3-9760-4B4BA3E1195B}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -423,15 +423,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>104774</xdr:colOff>
+      <xdr:colOff>102869</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>544830</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -446,8 +446,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7467599" y="400049"/>
-          <a:ext cx="5316856" cy="4572001"/>
+          <a:off x="7465694" y="400049"/>
+          <a:ext cx="5322571" cy="4791076"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -611,9 +611,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -651,7 +651,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -757,7 +757,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -899,7 +899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -918,7 +918,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,7 +1034,7 @@
   <dimension ref="A1:V189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F157" sqref="F157"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Had to change SiteDateID on other Excel file, too
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.3_months-to-include-for-precip-normals-comparison.xlsx
+++ b/data/data-wrangling-intermediate/03.3_months-to-include-for-precip-normals-comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3393" documentId="8_{89B2EEDE-D508-4F25-B24C-4C204CBA613B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{600068E6-2B54-4047-80A6-DEAB794755CF}"/>
+  <xr:revisionPtr revIDLastSave="3397" documentId="8_{89B2EEDE-D508-4F25-B24C-4C204CBA613B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28678E8F-E229-4CFF-89C4-8ECE709DAF0F}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{1028A4EE-DCCB-47E3-9760-4B4BA3E1195B}"/>
   </bookViews>
@@ -43,7 +43,7 @@
     <author>tc={2BC45058-0975-4BEF-AE3C-8CA9D07F3E25}</author>
   </authors>
   <commentList>
-    <comment ref="H154" authorId="0" shapeId="0" xr:uid="{2BC45058-0975-4BEF-AE3C-8CA9D07F3E25}">
+    <comment ref="H153" authorId="0" shapeId="0" xr:uid="{2BC45058-0975-4BEF-AE3C-8CA9D07F3E25}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1573" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="76">
   <si>
     <t>Region</t>
   </si>
@@ -385,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -401,6 +401,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -907,7 +908,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="H154" dT="2023-10-19T02:08:15.34" personId="{130D60B1-DC92-4EC1-B89C-690B1CF2E971}" id="{2BC45058-0975-4BEF-AE3C-8CA9D07F3E25}">
+  <threadedComment ref="H153" dT="2023-10-19T02:08:15.34" personId="{130D60B1-DC92-4EC1-B89C-690B1CF2E971}" id="{2BC45058-0975-4BEF-AE3C-8CA9D07F3E25}">
     <text>Will call this March.5 because the other date in same monitoring session (spring 2021) is March.5</text>
   </threadedComment>
 </ThreadedComments>
@@ -1031,11 +1032,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314917C4-A3F7-4522-885F-2395A80BBF8D}">
-  <dimension ref="A1:V189"/>
+  <dimension ref="A1:V188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F157" sqref="F157"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C188" activeCellId="10" sqref="C115 C120 C126 C131 C136 C140 C149 C161 C171 C180 C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5481,7 +5482,7 @@
       <c r="B115" t="s">
         <v>17</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="13">
         <v>114</v>
       </c>
       <c r="D115" s="6">
@@ -5520,50 +5521,38 @@
       </c>
     </row>
     <row r="116" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
+      <c r="A116" t="s">
         <v>16</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C116" s="2">
+      <c r="B116" t="s">
+        <v>18</v>
+      </c>
+      <c r="C116">
+        <f>C115+1</f>
         <v>115</v>
       </c>
-      <c r="D116" s="7">
-        <v>43903</v>
-      </c>
-      <c r="E116" s="3" t="s">
+      <c r="D116" s="6">
+        <v>43907</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F116" s="8">
+      <c r="F116" s="1">
         <v>43905</v>
       </c>
-      <c r="G116" s="7">
-        <v>44666</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I116" s="3">
-        <v>44666</v>
-      </c>
-      <c r="J116" s="9">
-        <v>1</v>
-      </c>
-      <c r="K116" s="2"/>
-      <c r="L116" s="2"/>
-      <c r="M116" s="2"/>
-      <c r="N116" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O116" s="2"/>
-      <c r="P116" s="2"/>
-      <c r="Q116" s="2"/>
-      <c r="R116" s="2"/>
-      <c r="S116" s="2"/>
-      <c r="T116" s="2"/>
-      <c r="U116" s="2"/>
-      <c r="V116" s="2"/>
+      <c r="G116" s="6">
+        <v>43951</v>
+      </c>
+      <c r="H116" t="s">
+        <v>34</v>
+      </c>
+      <c r="I116" s="1">
+        <v>43951</v>
+      </c>
+      <c r="J116" s="5"/>
+      <c r="N116">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="117" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
@@ -5573,6 +5562,7 @@
         <v>18</v>
       </c>
       <c r="C117">
+        <f t="shared" ref="C117:C180" si="0">C116+1</f>
         <v>116</v>
       </c>
       <c r="D117" s="6">
@@ -5585,17 +5575,50 @@
         <v>43905</v>
       </c>
       <c r="G117" s="6">
-        <v>43951</v>
+        <v>44292</v>
       </c>
       <c r="H117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I117" s="1">
-        <v>43951</v>
+        <v>44286</v>
       </c>
       <c r="J117" s="5"/>
+      <c r="K117">
+        <v>1</v>
+      </c>
+      <c r="L117">
+        <v>1</v>
+      </c>
+      <c r="M117">
+        <v>1</v>
+      </c>
       <c r="N117">
         <v>0.5</v>
+      </c>
+      <c r="O117">
+        <v>1</v>
+      </c>
+      <c r="P117">
+        <v>1</v>
+      </c>
+      <c r="Q117">
+        <v>1</v>
+      </c>
+      <c r="R117">
+        <v>1</v>
+      </c>
+      <c r="S117">
+        <v>1</v>
+      </c>
+      <c r="T117">
+        <v>1</v>
+      </c>
+      <c r="U117">
+        <v>1</v>
+      </c>
+      <c r="V117">
+        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.3">
@@ -5606,29 +5629,30 @@
         <v>18</v>
       </c>
       <c r="C118">
+        <f t="shared" si="0"/>
         <v>117</v>
       </c>
       <c r="D118" s="6">
-        <v>43907</v>
+        <v>44578</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F118" s="1">
-        <v>43905</v>
+        <v>44576</v>
       </c>
       <c r="G118" s="6">
-        <v>44292</v>
+        <v>44664</v>
       </c>
       <c r="H118" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I118" s="1">
-        <v>44286</v>
+        <v>44666</v>
       </c>
       <c r="J118" s="5"/>
       <c r="K118">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L118">
         <v>1</v>
@@ -5638,30 +5662,6 @@
       </c>
       <c r="N118">
         <v>0.5</v>
-      </c>
-      <c r="O118">
-        <v>1</v>
-      </c>
-      <c r="P118">
-        <v>1</v>
-      </c>
-      <c r="Q118">
-        <v>1</v>
-      </c>
-      <c r="R118">
-        <v>1</v>
-      </c>
-      <c r="S118">
-        <v>1</v>
-      </c>
-      <c r="T118">
-        <v>1</v>
-      </c>
-      <c r="U118">
-        <v>1</v>
-      </c>
-      <c r="V118">
-        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:22" x14ac:dyDescent="0.3">
@@ -5672,10 +5672,11 @@
         <v>18</v>
       </c>
       <c r="C119">
+        <f t="shared" si="0"/>
         <v>118</v>
       </c>
       <c r="D119" s="6">
-        <v>44578</v>
+        <v>44576</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>63</v>
@@ -5707,92 +5708,94 @@
       </c>
     </row>
     <row r="120" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="A120" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="13">
+        <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="D120" s="6">
-        <v>44576</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F120" s="1">
-        <v>44576</v>
-      </c>
-      <c r="G120" s="6">
+      <c r="D120" s="7">
+        <v>43907</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F120" s="8">
+        <v>43905</v>
+      </c>
+      <c r="G120" s="7">
         <v>44664</v>
       </c>
-      <c r="H120" t="s">
+      <c r="H120" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I120" s="1">
+      <c r="I120" s="8">
         <v>44666</v>
       </c>
-      <c r="J120" s="5"/>
-      <c r="K120">
-        <v>0.5</v>
-      </c>
-      <c r="L120">
-        <v>1</v>
-      </c>
-      <c r="M120">
-        <v>1</v>
-      </c>
-      <c r="N120">
-        <v>0.5</v>
-      </c>
+      <c r="J120" s="9">
+        <v>1</v>
+      </c>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2"/>
+      <c r="N120" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="O120" s="2"/>
+      <c r="P120" s="2"/>
+      <c r="Q120" s="2"/>
+      <c r="R120" s="2"/>
+      <c r="S120" s="2"/>
+      <c r="T120" s="2"/>
+      <c r="U120" s="2"/>
+      <c r="V120" s="2"/>
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C121" s="2">
+      <c r="A121" t="s">
+        <v>19</v>
+      </c>
+      <c r="B121" t="s">
+        <v>20</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="D121" s="7">
-        <v>43907</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F121" s="8">
-        <v>43905</v>
-      </c>
-      <c r="G121" s="7">
-        <v>44664</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I121" s="8">
-        <v>44666</v>
-      </c>
-      <c r="J121" s="9">
-        <v>1</v>
-      </c>
-      <c r="K121" s="2"/>
-      <c r="L121" s="2"/>
-      <c r="M121" s="2"/>
-      <c r="N121" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O121" s="2"/>
-      <c r="P121" s="2"/>
-      <c r="Q121" s="2"/>
-      <c r="R121" s="2"/>
-      <c r="S121" s="2"/>
-      <c r="T121" s="2"/>
-      <c r="U121" s="2"/>
-      <c r="V121" s="2"/>
+      <c r="D121" s="6">
+        <v>43818</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F121" s="1">
+        <v>43814</v>
+      </c>
+      <c r="G121" s="6">
+        <v>43920</v>
+      </c>
+      <c r="H121" t="s">
+        <v>33</v>
+      </c>
+      <c r="I121" s="1">
+        <v>43920</v>
+      </c>
+      <c r="J121" s="5"/>
+      <c r="K121">
+        <v>1</v>
+      </c>
+      <c r="L121">
+        <v>1</v>
+      </c>
+      <c r="M121">
+        <v>1</v>
+      </c>
+      <c r="V121">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="122" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
@@ -5802,6 +5805,7 @@
         <v>20</v>
       </c>
       <c r="C122">
+        <f t="shared" si="0"/>
         <v>121</v>
       </c>
       <c r="D122" s="6">
@@ -5814,25 +5818,34 @@
         <v>43814</v>
       </c>
       <c r="G122" s="6">
-        <v>43920</v>
+        <v>44118</v>
       </c>
       <c r="H122" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="I122" s="1">
-        <v>43920</v>
+        <v>44119</v>
       </c>
       <c r="J122" s="5"/>
-      <c r="K122">
-        <v>1</v>
-      </c>
-      <c r="L122">
-        <v>1</v>
-      </c>
-      <c r="M122">
-        <v>1</v>
-      </c>
-      <c r="V122">
+      <c r="N122">
+        <v>1</v>
+      </c>
+      <c r="O122">
+        <v>1</v>
+      </c>
+      <c r="P122">
+        <v>1</v>
+      </c>
+      <c r="Q122">
+        <v>1</v>
+      </c>
+      <c r="R122">
+        <v>1</v>
+      </c>
+      <c r="S122">
+        <v>1</v>
+      </c>
+      <c r="T122">
         <v>0.5</v>
       </c>
     </row>
@@ -5844,6 +5857,7 @@
         <v>20</v>
       </c>
       <c r="C123">
+        <f t="shared" si="0"/>
         <v>122</v>
       </c>
       <c r="D123" s="6">
@@ -5856,35 +5870,32 @@
         <v>43814</v>
       </c>
       <c r="G123" s="6">
-        <v>44118</v>
+        <v>44288</v>
       </c>
       <c r="H123" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I123" s="1">
-        <v>44119</v>
+        <v>44286</v>
       </c>
       <c r="J123" s="5"/>
-      <c r="N123">
-        <v>1</v>
-      </c>
-      <c r="O123">
-        <v>1</v>
-      </c>
-      <c r="P123">
-        <v>1</v>
-      </c>
-      <c r="Q123">
-        <v>1</v>
-      </c>
-      <c r="R123">
-        <v>1</v>
-      </c>
-      <c r="S123">
+      <c r="K123">
+        <v>1</v>
+      </c>
+      <c r="L123">
+        <v>1</v>
+      </c>
+      <c r="M123">
         <v>1</v>
       </c>
       <c r="T123">
         <v>0.5</v>
+      </c>
+      <c r="U123">
+        <v>1</v>
+      </c>
+      <c r="V123">
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:22" x14ac:dyDescent="0.3">
@@ -5895,6 +5906,7 @@
         <v>20</v>
       </c>
       <c r="C124">
+        <f t="shared" si="0"/>
         <v>123</v>
       </c>
       <c r="D124" s="6">
@@ -5907,31 +5919,31 @@
         <v>43814</v>
       </c>
       <c r="G124" s="6">
-        <v>44288</v>
+        <v>44473</v>
       </c>
       <c r="H124" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I124" s="1">
-        <v>44286</v>
+        <v>44469</v>
       </c>
       <c r="J124" s="5"/>
-      <c r="K124">
-        <v>1</v>
-      </c>
-      <c r="L124">
-        <v>1</v>
-      </c>
-      <c r="M124">
-        <v>1</v>
-      </c>
-      <c r="T124">
-        <v>0.5</v>
-      </c>
-      <c r="U124">
-        <v>1</v>
-      </c>
-      <c r="V124">
+      <c r="N124">
+        <v>1</v>
+      </c>
+      <c r="O124">
+        <v>1</v>
+      </c>
+      <c r="P124">
+        <v>1</v>
+      </c>
+      <c r="Q124">
+        <v>1</v>
+      </c>
+      <c r="R124">
+        <v>1</v>
+      </c>
+      <c r="S124">
         <v>1</v>
       </c>
     </row>
@@ -5943,6 +5955,7 @@
         <v>20</v>
       </c>
       <c r="C125">
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="D125" s="6">
@@ -5955,125 +5968,121 @@
         <v>43814</v>
       </c>
       <c r="G125" s="6">
-        <v>44473</v>
+        <v>44649</v>
       </c>
       <c r="H125" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I125" s="1">
-        <v>44469</v>
+        <v>44651</v>
       </c>
       <c r="J125" s="5"/>
-      <c r="N125">
-        <v>1</v>
-      </c>
-      <c r="O125">
-        <v>1</v>
-      </c>
-      <c r="P125">
-        <v>1</v>
-      </c>
-      <c r="Q125">
-        <v>1</v>
-      </c>
-      <c r="R125">
-        <v>1</v>
-      </c>
-      <c r="S125">
+      <c r="K125">
+        <v>1</v>
+      </c>
+      <c r="L125">
+        <v>1</v>
+      </c>
+      <c r="M125">
+        <v>1</v>
+      </c>
+      <c r="T125">
+        <v>1</v>
+      </c>
+      <c r="U125">
+        <v>1</v>
+      </c>
+      <c r="V125">
         <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="A126" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="13">
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D126" s="7">
         <v>43818</v>
       </c>
-      <c r="E126" s="1" t="s">
+      <c r="E126" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F126" s="1">
+      <c r="F126" s="8">
         <v>43814</v>
       </c>
-      <c r="G126" s="6">
-        <v>44649</v>
-      </c>
-      <c r="H126" t="s">
+      <c r="G126" s="7">
+        <v>45009</v>
+      </c>
+      <c r="H126" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I126" s="1">
-        <v>44651</v>
-      </c>
-      <c r="J126" s="5"/>
-      <c r="K126">
-        <v>1</v>
-      </c>
-      <c r="L126">
-        <v>1</v>
-      </c>
-      <c r="M126">
-        <v>1</v>
-      </c>
-      <c r="T126">
-        <v>1</v>
-      </c>
-      <c r="U126">
-        <v>1</v>
-      </c>
-      <c r="V126">
-        <v>1</v>
-      </c>
+      <c r="I126" s="3">
+        <v>45016</v>
+      </c>
+      <c r="J126" s="9">
+        <v>1</v>
+      </c>
+      <c r="K126" s="2"/>
+      <c r="L126" s="2"/>
+      <c r="M126" s="2"/>
+      <c r="N126" s="2"/>
+      <c r="O126" s="2"/>
+      <c r="P126" s="2"/>
+      <c r="Q126" s="2"/>
+      <c r="R126" s="2"/>
+      <c r="S126" s="2"/>
+      <c r="T126" s="2"/>
+      <c r="U126" s="2"/>
+      <c r="V126" s="2"/>
     </row>
     <row r="127" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
+      <c r="A127" t="s">
         <v>19</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C127" s="2">
+      <c r="B127" t="s">
+        <v>21</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="D127" s="7">
-        <v>43818</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F127" s="8">
-        <v>43814</v>
-      </c>
-      <c r="G127" s="7">
-        <v>45009</v>
-      </c>
-      <c r="H127" s="2" t="s">
+      <c r="D127" s="6">
+        <v>43794</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F127" s="1">
+        <v>43800</v>
+      </c>
+      <c r="G127" s="6">
+        <v>43916</v>
+      </c>
+      <c r="H127" t="s">
         <v>33</v>
       </c>
-      <c r="I127" s="3">
-        <v>45016</v>
-      </c>
-      <c r="J127" s="9">
-        <v>1</v>
-      </c>
-      <c r="K127" s="2"/>
-      <c r="L127" s="2"/>
-      <c r="M127" s="2"/>
-      <c r="N127" s="2"/>
-      <c r="O127" s="2"/>
-      <c r="P127" s="2"/>
-      <c r="Q127" s="2"/>
-      <c r="R127" s="2"/>
-      <c r="S127" s="2"/>
-      <c r="T127" s="2"/>
-      <c r="U127" s="2"/>
-      <c r="V127" s="2"/>
+      <c r="I127" s="1">
+        <v>43920</v>
+      </c>
+      <c r="J127" s="5"/>
+      <c r="K127">
+        <v>1</v>
+      </c>
+      <c r="L127">
+        <v>1</v>
+      </c>
+      <c r="M127">
+        <v>1</v>
+      </c>
+      <c r="V127">
+        <v>1</v>
+      </c>
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
@@ -6083,6 +6092,7 @@
         <v>21</v>
       </c>
       <c r="C128">
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="D128" s="6">
@@ -6095,26 +6105,35 @@
         <v>43800</v>
       </c>
       <c r="G128" s="6">
-        <v>43916</v>
+        <v>44116</v>
       </c>
       <c r="H128" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="I128" s="1">
-        <v>43920</v>
+        <v>44119</v>
       </c>
       <c r="J128" s="5"/>
-      <c r="K128">
-        <v>1</v>
-      </c>
-      <c r="L128">
-        <v>1</v>
-      </c>
-      <c r="M128">
-        <v>1</v>
-      </c>
-      <c r="V128">
-        <v>1</v>
+      <c r="N128">
+        <v>1</v>
+      </c>
+      <c r="O128">
+        <v>1</v>
+      </c>
+      <c r="P128">
+        <v>1</v>
+      </c>
+      <c r="Q128">
+        <v>1</v>
+      </c>
+      <c r="R128">
+        <v>1</v>
+      </c>
+      <c r="S128">
+        <v>1</v>
+      </c>
+      <c r="T128">
+        <v>0.5</v>
       </c>
     </row>
     <row r="129" spans="1:22" x14ac:dyDescent="0.3">
@@ -6125,6 +6144,7 @@
         <v>21</v>
       </c>
       <c r="C129">
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="D129" s="6">
@@ -6137,35 +6157,32 @@
         <v>43800</v>
       </c>
       <c r="G129" s="6">
-        <v>44116</v>
+        <v>44285</v>
       </c>
       <c r="H129" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I129" s="1">
-        <v>44119</v>
+        <v>44286</v>
       </c>
       <c r="J129" s="5"/>
-      <c r="N129">
-        <v>1</v>
-      </c>
-      <c r="O129">
-        <v>1</v>
-      </c>
-      <c r="P129">
-        <v>1</v>
-      </c>
-      <c r="Q129">
-        <v>1</v>
-      </c>
-      <c r="R129">
-        <v>1</v>
-      </c>
-      <c r="S129">
+      <c r="K129">
+        <v>1</v>
+      </c>
+      <c r="L129">
+        <v>1</v>
+      </c>
+      <c r="M129">
         <v>1</v>
       </c>
       <c r="T129">
         <v>0.5</v>
+      </c>
+      <c r="U129">
+        <v>1</v>
+      </c>
+      <c r="V129">
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:22" x14ac:dyDescent="0.3">
@@ -6176,6 +6193,7 @@
         <v>21</v>
       </c>
       <c r="C130">
+        <f t="shared" si="0"/>
         <v>129</v>
       </c>
       <c r="D130" s="6">
@@ -6188,133 +6206,129 @@
         <v>43800</v>
       </c>
       <c r="G130" s="6">
-        <v>44285</v>
+        <v>44475</v>
       </c>
       <c r="H130" t="s">
+        <v>39</v>
+      </c>
+      <c r="I130" s="1">
+        <v>44469</v>
+      </c>
+      <c r="J130" s="5"/>
+      <c r="N130">
+        <v>1</v>
+      </c>
+      <c r="O130">
+        <v>1</v>
+      </c>
+      <c r="P130">
+        <v>1</v>
+      </c>
+      <c r="Q130">
+        <v>1</v>
+      </c>
+      <c r="R130">
+        <v>1</v>
+      </c>
+      <c r="S130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C131" s="13">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="D131" s="7">
+        <v>43794</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F131" s="8">
+        <v>43800</v>
+      </c>
+      <c r="G131" s="7">
+        <v>44651</v>
+      </c>
+      <c r="H131" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I130" s="1">
-        <v>44286</v>
-      </c>
-      <c r="J130" s="5"/>
-      <c r="K130">
-        <v>1</v>
-      </c>
-      <c r="L130">
-        <v>1</v>
-      </c>
-      <c r="M130">
-        <v>1</v>
-      </c>
-      <c r="T130">
-        <v>0.5</v>
-      </c>
-      <c r="U130">
-        <v>1</v>
-      </c>
-      <c r="V130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+      <c r="I131" s="3">
+        <v>44651</v>
+      </c>
+      <c r="J131" s="9"/>
+      <c r="K131" s="2">
+        <v>1</v>
+      </c>
+      <c r="L131" s="2">
+        <v>1</v>
+      </c>
+      <c r="M131" s="2">
+        <v>1</v>
+      </c>
+      <c r="N131" s="2"/>
+      <c r="O131" s="2"/>
+      <c r="P131" s="2"/>
+      <c r="Q131" s="2"/>
+      <c r="R131" s="2"/>
+      <c r="S131" s="2"/>
+      <c r="T131" s="2">
+        <v>1</v>
+      </c>
+      <c r="U131" s="2">
+        <v>1</v>
+      </c>
+      <c r="V131" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>19</v>
       </c>
-      <c r="B131" t="s">
-        <v>21</v>
-      </c>
-      <c r="C131">
-        <v>130</v>
-      </c>
-      <c r="D131" s="6">
-        <v>43794</v>
-      </c>
-      <c r="E131" s="1" t="s">
+      <c r="B132" t="s">
+        <v>22</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="D132" s="6">
+        <v>43791</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F131" s="1">
+      <c r="F132" s="1">
         <v>43800</v>
       </c>
-      <c r="G131" s="6">
-        <v>44475</v>
-      </c>
-      <c r="H131" t="s">
-        <v>39</v>
-      </c>
-      <c r="I131" s="1">
-        <v>44469</v>
-      </c>
-      <c r="J131" s="5"/>
-      <c r="N131">
-        <v>1</v>
-      </c>
-      <c r="O131">
-        <v>1</v>
-      </c>
-      <c r="P131">
-        <v>1</v>
-      </c>
-      <c r="Q131">
-        <v>1</v>
-      </c>
-      <c r="R131">
-        <v>1</v>
-      </c>
-      <c r="S131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C132" s="2">
-        <v>131</v>
-      </c>
-      <c r="D132" s="7">
-        <v>43794</v>
-      </c>
-      <c r="E132" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F132" s="8">
-        <v>43800</v>
-      </c>
-      <c r="G132" s="7">
-        <v>44651</v>
-      </c>
-      <c r="H132" s="2" t="s">
+      <c r="G132" s="6">
+        <v>43915</v>
+      </c>
+      <c r="H132" t="s">
         <v>33</v>
       </c>
-      <c r="I132" s="3">
-        <v>44651</v>
-      </c>
-      <c r="J132" s="9"/>
-      <c r="K132" s="2">
-        <v>1</v>
-      </c>
-      <c r="L132" s="2">
-        <v>1</v>
-      </c>
-      <c r="M132" s="2">
-        <v>1</v>
-      </c>
-      <c r="N132" s="2"/>
-      <c r="O132" s="2"/>
-      <c r="P132" s="2"/>
-      <c r="Q132" s="2"/>
-      <c r="R132" s="2"/>
-      <c r="S132" s="2"/>
-      <c r="T132" s="2">
-        <v>1</v>
-      </c>
-      <c r="U132" s="2">
-        <v>1</v>
-      </c>
-      <c r="V132" s="2">
+      <c r="I132" s="1">
+        <v>43920</v>
+      </c>
+      <c r="J132" s="5"/>
+      <c r="K132">
+        <v>1</v>
+      </c>
+      <c r="L132">
+        <v>1</v>
+      </c>
+      <c r="M132">
+        <v>1</v>
+      </c>
+      <c r="V132">
         <v>1</v>
       </c>
     </row>
@@ -6326,6 +6340,7 @@
         <v>22</v>
       </c>
       <c r="C133">
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="D133" s="6">
@@ -6338,26 +6353,35 @@
         <v>43800</v>
       </c>
       <c r="G133" s="6">
-        <v>43915</v>
+        <v>44119</v>
       </c>
       <c r="H133" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="I133" s="1">
-        <v>43920</v>
+        <v>44119</v>
       </c>
       <c r="J133" s="5"/>
-      <c r="K133">
-        <v>1</v>
-      </c>
-      <c r="L133">
-        <v>1</v>
-      </c>
-      <c r="M133">
-        <v>1</v>
-      </c>
-      <c r="V133">
-        <v>1</v>
+      <c r="N133">
+        <v>1</v>
+      </c>
+      <c r="O133">
+        <v>1</v>
+      </c>
+      <c r="P133">
+        <v>1</v>
+      </c>
+      <c r="Q133">
+        <v>1</v>
+      </c>
+      <c r="R133">
+        <v>1</v>
+      </c>
+      <c r="S133">
+        <v>1</v>
+      </c>
+      <c r="T133">
+        <v>0.5</v>
       </c>
     </row>
     <row r="134" spans="1:22" x14ac:dyDescent="0.3">
@@ -6368,6 +6392,7 @@
         <v>22</v>
       </c>
       <c r="C134">
+        <f t="shared" si="0"/>
         <v>133</v>
       </c>
       <c r="D134" s="6">
@@ -6380,35 +6405,32 @@
         <v>43800</v>
       </c>
       <c r="G134" s="6">
-        <v>44119</v>
+        <v>44287</v>
       </c>
       <c r="H134" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I134" s="1">
-        <v>44119</v>
+        <v>44286</v>
       </c>
       <c r="J134" s="5"/>
-      <c r="N134">
-        <v>1</v>
-      </c>
-      <c r="O134">
-        <v>1</v>
-      </c>
-      <c r="P134">
-        <v>1</v>
-      </c>
-      <c r="Q134">
-        <v>1</v>
-      </c>
-      <c r="R134">
-        <v>1</v>
-      </c>
-      <c r="S134">
+      <c r="K134">
+        <v>1</v>
+      </c>
+      <c r="L134">
+        <v>1</v>
+      </c>
+      <c r="M134">
         <v>1</v>
       </c>
       <c r="T134">
         <v>0.5</v>
+      </c>
+      <c r="U134">
+        <v>1</v>
+      </c>
+      <c r="V134">
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:22" x14ac:dyDescent="0.3">
@@ -6419,6 +6441,7 @@
         <v>22</v>
       </c>
       <c r="C135">
+        <f t="shared" si="0"/>
         <v>134</v>
       </c>
       <c r="D135" s="6">
@@ -6431,133 +6454,129 @@
         <v>43800</v>
       </c>
       <c r="G135" s="6">
-        <v>44287</v>
+        <v>44477</v>
       </c>
       <c r="H135" t="s">
+        <v>39</v>
+      </c>
+      <c r="I135" s="1">
+        <v>44469</v>
+      </c>
+      <c r="J135" s="5"/>
+      <c r="N135">
+        <v>1</v>
+      </c>
+      <c r="O135">
+        <v>1</v>
+      </c>
+      <c r="P135">
+        <v>1</v>
+      </c>
+      <c r="Q135">
+        <v>1</v>
+      </c>
+      <c r="R135">
+        <v>1</v>
+      </c>
+      <c r="S135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C136" s="13">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="D136" s="7">
+        <v>43791</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F136" s="8">
+        <v>43800</v>
+      </c>
+      <c r="G136" s="7">
+        <v>44648</v>
+      </c>
+      <c r="H136" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I135" s="1">
-        <v>44286</v>
-      </c>
-      <c r="J135" s="5"/>
-      <c r="K135">
-        <v>1</v>
-      </c>
-      <c r="L135">
-        <v>1</v>
-      </c>
-      <c r="M135">
-        <v>1</v>
-      </c>
-      <c r="T135">
-        <v>0.5</v>
-      </c>
-      <c r="U135">
-        <v>1</v>
-      </c>
-      <c r="V135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+      <c r="I136" s="3">
+        <v>44651</v>
+      </c>
+      <c r="J136" s="9"/>
+      <c r="K136" s="2">
+        <v>1</v>
+      </c>
+      <c r="L136" s="2">
+        <v>1</v>
+      </c>
+      <c r="M136" s="2">
+        <v>1</v>
+      </c>
+      <c r="N136" s="2"/>
+      <c r="O136" s="2"/>
+      <c r="P136" s="2"/>
+      <c r="Q136" s="2"/>
+      <c r="R136" s="2"/>
+      <c r="S136" s="2"/>
+      <c r="T136" s="2">
+        <v>1</v>
+      </c>
+      <c r="U136" s="2">
+        <v>1</v>
+      </c>
+      <c r="V136" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>19</v>
       </c>
-      <c r="B136" t="s">
-        <v>22</v>
-      </c>
-      <c r="C136">
-        <v>135</v>
-      </c>
-      <c r="D136" s="6">
-        <v>43791</v>
-      </c>
-      <c r="E136" s="1" t="s">
+      <c r="B137" t="s">
+        <v>23</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="D137" s="6">
+        <v>43790</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F136" s="1">
+      <c r="F137" s="1">
         <v>43800</v>
       </c>
-      <c r="G136" s="6">
-        <v>44477</v>
-      </c>
-      <c r="H136" t="s">
-        <v>39</v>
-      </c>
-      <c r="I136" s="1">
-        <v>44469</v>
-      </c>
-      <c r="J136" s="5"/>
-      <c r="N136">
-        <v>1</v>
-      </c>
-      <c r="O136">
-        <v>1</v>
-      </c>
-      <c r="P136">
-        <v>1</v>
-      </c>
-      <c r="Q136">
-        <v>1</v>
-      </c>
-      <c r="R136">
-        <v>1</v>
-      </c>
-      <c r="S136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C137" s="2">
-        <v>136</v>
-      </c>
-      <c r="D137" s="7">
-        <v>43791</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F137" s="8">
-        <v>43800</v>
-      </c>
-      <c r="G137" s="7">
-        <v>44648</v>
-      </c>
-      <c r="H137" s="2" t="s">
+      <c r="G137" s="6">
+        <v>43917</v>
+      </c>
+      <c r="H137" t="s">
         <v>33</v>
       </c>
-      <c r="I137" s="3">
-        <v>44651</v>
-      </c>
-      <c r="J137" s="9"/>
-      <c r="K137" s="2">
-        <v>1</v>
-      </c>
-      <c r="L137" s="2">
-        <v>1</v>
-      </c>
-      <c r="M137" s="2">
-        <v>1</v>
-      </c>
-      <c r="N137" s="2"/>
-      <c r="O137" s="2"/>
-      <c r="P137" s="2"/>
-      <c r="Q137" s="2"/>
-      <c r="R137" s="2"/>
-      <c r="S137" s="2"/>
-      <c r="T137" s="2">
-        <v>1</v>
-      </c>
-      <c r="U137" s="2">
-        <v>1</v>
-      </c>
-      <c r="V137" s="2">
+      <c r="I137" s="1">
+        <v>43920</v>
+      </c>
+      <c r="J137" s="5"/>
+      <c r="K137">
+        <v>1</v>
+      </c>
+      <c r="L137">
+        <v>1</v>
+      </c>
+      <c r="M137">
+        <v>1</v>
+      </c>
+      <c r="V137">
         <v>1</v>
       </c>
     </row>
@@ -6569,6 +6588,7 @@
         <v>23</v>
       </c>
       <c r="C138">
+        <f t="shared" si="0"/>
         <v>137</v>
       </c>
       <c r="D138" s="6">
@@ -6581,26 +6601,35 @@
         <v>43800</v>
       </c>
       <c r="G138" s="6">
-        <v>43917</v>
+        <v>44117</v>
       </c>
       <c r="H138" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="I138" s="1">
-        <v>43920</v>
+        <v>44119</v>
       </c>
       <c r="J138" s="5"/>
-      <c r="K138">
-        <v>1</v>
-      </c>
-      <c r="L138">
-        <v>1</v>
-      </c>
-      <c r="M138">
-        <v>1</v>
-      </c>
-      <c r="V138">
-        <v>1</v>
+      <c r="N138">
+        <v>1</v>
+      </c>
+      <c r="O138">
+        <v>1</v>
+      </c>
+      <c r="P138">
+        <v>1</v>
+      </c>
+      <c r="Q138">
+        <v>1</v>
+      </c>
+      <c r="R138">
+        <v>1</v>
+      </c>
+      <c r="S138">
+        <v>1</v>
+      </c>
+      <c r="T138">
+        <v>0.5</v>
       </c>
     </row>
     <row r="139" spans="1:22" x14ac:dyDescent="0.3">
@@ -6611,6 +6640,7 @@
         <v>23</v>
       </c>
       <c r="C139">
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
       <c r="D139" s="6">
@@ -6623,140 +6653,130 @@
         <v>43800</v>
       </c>
       <c r="G139" s="6">
-        <v>44117</v>
+        <v>44286</v>
       </c>
       <c r="H139" t="s">
+        <v>33</v>
+      </c>
+      <c r="I139" s="1">
+        <v>44286</v>
+      </c>
+      <c r="J139" s="5"/>
+      <c r="K139">
+        <v>1</v>
+      </c>
+      <c r="L139">
+        <v>1</v>
+      </c>
+      <c r="M139">
+        <v>1</v>
+      </c>
+      <c r="T139">
+        <v>0.5</v>
+      </c>
+      <c r="U139">
+        <v>1</v>
+      </c>
+      <c r="V139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C140" s="13">
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="D140" s="7">
+        <v>43790</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F140" s="8">
+        <v>43800</v>
+      </c>
+      <c r="G140" s="7">
+        <v>44482</v>
+      </c>
+      <c r="H140" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I139" s="1">
-        <v>44119</v>
-      </c>
-      <c r="J139" s="5"/>
-      <c r="N139">
-        <v>1</v>
-      </c>
-      <c r="O139">
-        <v>1</v>
-      </c>
-      <c r="P139">
-        <v>1</v>
-      </c>
-      <c r="Q139">
-        <v>1</v>
-      </c>
-      <c r="R139">
-        <v>1</v>
-      </c>
-      <c r="S139">
-        <v>1</v>
-      </c>
-      <c r="T139">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>19</v>
-      </c>
-      <c r="B140" t="s">
-        <v>23</v>
-      </c>
-      <c r="C140">
-        <v>139</v>
-      </c>
-      <c r="D140" s="6">
-        <v>43790</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F140" s="1">
-        <v>43800</v>
-      </c>
-      <c r="G140" s="6">
-        <v>44286</v>
-      </c>
-      <c r="H140" t="s">
-        <v>33</v>
-      </c>
-      <c r="I140" s="1">
-        <v>44286</v>
-      </c>
-      <c r="J140" s="5"/>
-      <c r="K140">
-        <v>1</v>
-      </c>
-      <c r="L140">
-        <v>1</v>
-      </c>
-      <c r="M140">
-        <v>1</v>
-      </c>
-      <c r="T140">
-        <v>0.5</v>
-      </c>
-      <c r="U140">
-        <v>1</v>
-      </c>
-      <c r="V140">
-        <v>1</v>
-      </c>
+      <c r="I140" s="3">
+        <v>44484</v>
+      </c>
+      <c r="J140" s="9"/>
+      <c r="K140" s="2"/>
+      <c r="L140" s="2"/>
+      <c r="M140" s="2"/>
+      <c r="N140" s="2">
+        <v>1</v>
+      </c>
+      <c r="O140" s="2">
+        <v>1</v>
+      </c>
+      <c r="P140" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q140" s="2">
+        <v>1</v>
+      </c>
+      <c r="R140" s="2">
+        <v>1</v>
+      </c>
+      <c r="S140" s="2">
+        <v>1</v>
+      </c>
+      <c r="T140" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="U140" s="2"/>
+      <c r="V140" s="2"/>
     </row>
     <row r="141" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C141" s="2">
+      <c r="A141" t="s">
+        <v>24</v>
+      </c>
+      <c r="B141" t="s">
+        <v>25</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="D141" s="7">
-        <v>43790</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F141" s="8">
-        <v>43800</v>
-      </c>
-      <c r="G141" s="7">
-        <v>44482</v>
-      </c>
-      <c r="H141" s="2" t="s">
+      <c r="D141" s="6">
+        <v>43686</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F141" s="1">
+        <v>43678</v>
+      </c>
+      <c r="G141" s="6">
+        <v>43781</v>
+      </c>
+      <c r="H141" t="s">
         <v>64</v>
       </c>
-      <c r="I141" s="3">
-        <v>44484</v>
-      </c>
-      <c r="J141" s="9"/>
-      <c r="K141" s="2"/>
-      <c r="L141" s="2"/>
-      <c r="M141" s="2"/>
-      <c r="N141" s="2">
-        <v>1</v>
-      </c>
-      <c r="O141" s="2">
-        <v>1</v>
-      </c>
-      <c r="P141" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q141" s="2">
-        <v>1</v>
-      </c>
-      <c r="R141" s="2">
-        <v>1</v>
-      </c>
-      <c r="S141" s="2">
-        <v>1</v>
-      </c>
-      <c r="T141" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="U141" s="2"/>
-      <c r="V141" s="2"/>
+      <c r="I141" s="1">
+        <v>43753</v>
+      </c>
+      <c r="J141" s="5"/>
+      <c r="R141">
+        <v>1</v>
+      </c>
+      <c r="S141">
+        <v>1</v>
+      </c>
+      <c r="T141">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="142" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
@@ -6766,6 +6786,7 @@
         <v>25</v>
       </c>
       <c r="C142">
+        <f t="shared" si="0"/>
         <v>141</v>
       </c>
       <c r="D142" s="6">
@@ -6778,23 +6799,32 @@
         <v>43678</v>
       </c>
       <c r="G142" s="6">
-        <v>43781</v>
+        <v>43920</v>
       </c>
       <c r="H142" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I142" s="1">
-        <v>43753</v>
+        <v>43921</v>
       </c>
       <c r="J142" s="5"/>
-      <c r="R142">
-        <v>1</v>
-      </c>
-      <c r="S142">
+      <c r="K142">
+        <v>1</v>
+      </c>
+      <c r="L142">
+        <v>1</v>
+      </c>
+      <c r="M142">
         <v>1</v>
       </c>
       <c r="T142">
         <v>0.5</v>
+      </c>
+      <c r="U142">
+        <v>1</v>
+      </c>
+      <c r="V142">
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:22" x14ac:dyDescent="0.3">
@@ -6805,6 +6835,7 @@
         <v>25</v>
       </c>
       <c r="C143">
+        <f t="shared" si="0"/>
         <v>142</v>
       </c>
       <c r="D143" s="6">
@@ -6817,31 +6848,31 @@
         <v>43678</v>
       </c>
       <c r="G143" s="6">
-        <v>43920</v>
+        <v>44105</v>
       </c>
       <c r="H143" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I143" s="1">
-        <v>43921</v>
+        <v>44104</v>
       </c>
       <c r="J143" s="5"/>
-      <c r="K143">
-        <v>1</v>
-      </c>
-      <c r="L143">
-        <v>1</v>
-      </c>
-      <c r="M143">
-        <v>1</v>
-      </c>
-      <c r="T143">
-        <v>0.5</v>
-      </c>
-      <c r="U143">
-        <v>1</v>
-      </c>
-      <c r="V143">
+      <c r="N143">
+        <v>1</v>
+      </c>
+      <c r="O143">
+        <v>1</v>
+      </c>
+      <c r="P143">
+        <v>1</v>
+      </c>
+      <c r="Q143">
+        <v>1</v>
+      </c>
+      <c r="R143">
+        <v>1</v>
+      </c>
+      <c r="S143">
         <v>1</v>
       </c>
     </row>
@@ -6853,6 +6884,7 @@
         <v>25</v>
       </c>
       <c r="C144">
+        <f t="shared" si="0"/>
         <v>143</v>
       </c>
       <c r="D144" s="6">
@@ -6865,7 +6897,7 @@
         <v>43678</v>
       </c>
       <c r="G144" s="6">
-        <v>44105</v>
+        <v>44108</v>
       </c>
       <c r="H144" t="s">
         <v>39</v>
@@ -6901,6 +6933,7 @@
         <v>25</v>
       </c>
       <c r="C145">
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="D145" s="6">
@@ -6913,31 +6946,31 @@
         <v>43678</v>
       </c>
       <c r="G145" s="6">
-        <v>44108</v>
+        <v>44267</v>
       </c>
       <c r="H145" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="I145" s="1">
-        <v>44104</v>
+        <v>44270</v>
       </c>
       <c r="J145" s="5"/>
-      <c r="N145">
-        <v>1</v>
-      </c>
-      <c r="O145">
-        <v>1</v>
-      </c>
-      <c r="P145">
-        <v>1</v>
-      </c>
-      <c r="Q145">
-        <v>1</v>
-      </c>
-      <c r="R145">
-        <v>1</v>
-      </c>
-      <c r="S145">
+      <c r="K145">
+        <v>1</v>
+      </c>
+      <c r="L145">
+        <v>1</v>
+      </c>
+      <c r="M145">
+        <v>0.5</v>
+      </c>
+      <c r="T145">
+        <v>1</v>
+      </c>
+      <c r="U145">
+        <v>1</v>
+      </c>
+      <c r="V145">
         <v>1</v>
       </c>
     </row>
@@ -6949,6 +6982,7 @@
         <v>25</v>
       </c>
       <c r="C146">
+        <f t="shared" si="0"/>
         <v>145</v>
       </c>
       <c r="D146" s="6">
@@ -6961,32 +6995,38 @@
         <v>43678</v>
       </c>
       <c r="G146" s="6">
-        <v>44267</v>
+        <v>44482</v>
       </c>
       <c r="H146" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I146" s="1">
-        <v>44270</v>
+        <v>44484</v>
       </c>
       <c r="J146" s="5"/>
-      <c r="K146">
-        <v>1</v>
-      </c>
-      <c r="L146">
-        <v>1</v>
-      </c>
       <c r="M146">
         <v>0.5</v>
       </c>
+      <c r="N146">
+        <v>1</v>
+      </c>
+      <c r="O146">
+        <v>1</v>
+      </c>
+      <c r="P146">
+        <v>1</v>
+      </c>
+      <c r="Q146">
+        <v>1</v>
+      </c>
+      <c r="R146">
+        <v>1</v>
+      </c>
+      <c r="S146">
+        <v>1</v>
+      </c>
       <c r="T146">
-        <v>1</v>
-      </c>
-      <c r="U146">
-        <v>1</v>
-      </c>
-      <c r="V146">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="147" spans="1:22" x14ac:dyDescent="0.3">
@@ -6997,6 +7037,7 @@
         <v>25</v>
       </c>
       <c r="C147">
+        <f t="shared" si="0"/>
         <v>146</v>
       </c>
       <c r="D147" s="6">
@@ -7009,7 +7050,7 @@
         <v>43678</v>
       </c>
       <c r="G147" s="6">
-        <v>44482</v>
+        <v>44483</v>
       </c>
       <c r="H147" t="s">
         <v>64</v>
@@ -7051,6 +7092,7 @@
         <v>25</v>
       </c>
       <c r="C148">
+        <f t="shared" si="0"/>
         <v>147</v>
       </c>
       <c r="D148" s="6">
@@ -7063,140 +7105,127 @@
         <v>43678</v>
       </c>
       <c r="G148" s="6">
-        <v>44483</v>
+        <v>44650</v>
       </c>
       <c r="H148" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I148" s="1">
-        <v>44484</v>
+        <v>44651</v>
       </c>
       <c r="J148" s="5"/>
+      <c r="K148">
+        <v>1</v>
+      </c>
+      <c r="L148">
+        <v>1</v>
+      </c>
       <c r="M148">
-        <v>0.5</v>
-      </c>
-      <c r="N148">
-        <v>1</v>
-      </c>
-      <c r="O148">
-        <v>1</v>
-      </c>
-      <c r="P148">
-        <v>1</v>
-      </c>
-      <c r="Q148">
-        <v>1</v>
-      </c>
-      <c r="R148">
-        <v>1</v>
-      </c>
-      <c r="S148">
         <v>1</v>
       </c>
       <c r="T148">
         <v>0.5</v>
       </c>
+      <c r="U148">
+        <v>1</v>
+      </c>
+      <c r="V148">
+        <v>1</v>
+      </c>
     </row>
     <row r="149" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+      <c r="A149" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C149">
+      <c r="C149" s="13">
+        <f t="shared" si="0"/>
         <v>148</v>
       </c>
-      <c r="D149" s="6">
+      <c r="D149" s="7">
         <v>43686</v>
       </c>
-      <c r="E149" s="1" t="s">
+      <c r="E149" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F149" s="1">
+      <c r="F149" s="8">
         <v>43678</v>
       </c>
-      <c r="G149" s="6">
-        <v>44650</v>
-      </c>
-      <c r="H149" t="s">
+      <c r="G149" s="7">
+        <v>44651</v>
+      </c>
+      <c r="H149" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I149" s="1">
+      <c r="I149" s="3">
         <v>44651</v>
       </c>
-      <c r="J149" s="5"/>
-      <c r="K149">
-        <v>1</v>
-      </c>
-      <c r="L149">
-        <v>1</v>
-      </c>
-      <c r="M149">
-        <v>1</v>
-      </c>
-      <c r="T149">
-        <v>0.5</v>
-      </c>
-      <c r="U149">
-        <v>1</v>
-      </c>
-      <c r="V149">
+      <c r="J149" s="9"/>
+      <c r="K149" s="2">
+        <v>1</v>
+      </c>
+      <c r="L149" s="2">
+        <v>1</v>
+      </c>
+      <c r="M149" s="2">
+        <v>1</v>
+      </c>
+      <c r="N149" s="2"/>
+      <c r="O149" s="2"/>
+      <c r="P149" s="2"/>
+      <c r="Q149" s="2"/>
+      <c r="R149" s="2"/>
+      <c r="S149" s="2"/>
+      <c r="T149" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="U149" s="2">
+        <v>1</v>
+      </c>
+      <c r="V149" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
+      <c r="A150" t="s">
         <v>24</v>
       </c>
-      <c r="B150" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C150" s="2">
+      <c r="B150" t="s">
+        <v>26</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="0"/>
         <v>149</v>
       </c>
-      <c r="D150" s="7">
+      <c r="D150" s="6">
         <v>43686</v>
       </c>
-      <c r="E150" s="3" t="s">
+      <c r="E150" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F150" s="8">
+      <c r="F150" s="1">
         <v>43678</v>
       </c>
-      <c r="G150" s="7">
-        <v>44651</v>
-      </c>
-      <c r="H150" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I150" s="3">
-        <v>44651</v>
-      </c>
-      <c r="J150" s="9"/>
-      <c r="K150" s="2">
-        <v>1</v>
-      </c>
-      <c r="L150" s="2">
-        <v>1</v>
-      </c>
-      <c r="M150" s="2">
-        <v>1</v>
-      </c>
-      <c r="N150" s="2"/>
-      <c r="O150" s="2"/>
-      <c r="P150" s="2"/>
-      <c r="Q150" s="2"/>
-      <c r="R150" s="2"/>
-      <c r="S150" s="2"/>
-      <c r="T150" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="U150" s="2">
-        <v>1</v>
-      </c>
-      <c r="V150" s="2">
-        <v>1</v>
+      <c r="G150" s="6">
+        <v>43776</v>
+      </c>
+      <c r="H150" t="s">
+        <v>40</v>
+      </c>
+      <c r="I150" s="1">
+        <v>43769</v>
+      </c>
+      <c r="J150" s="5"/>
+      <c r="R150">
+        <v>1</v>
+      </c>
+      <c r="S150">
+        <v>1</v>
+      </c>
+      <c r="T150">
+        <v>0.5</v>
       </c>
     </row>
     <row r="151" spans="1:22" x14ac:dyDescent="0.3">
@@ -7207,6 +7236,7 @@
         <v>26</v>
       </c>
       <c r="C151">
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D151" s="6">
@@ -7219,23 +7249,32 @@
         <v>43678</v>
       </c>
       <c r="G151" s="6">
-        <v>43776</v>
+        <v>43923</v>
       </c>
       <c r="H151" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I151" s="1">
-        <v>43769</v>
+        <v>43921</v>
       </c>
       <c r="J151" s="5"/>
-      <c r="R151">
-        <v>1</v>
-      </c>
-      <c r="S151">
+      <c r="K151">
+        <v>1</v>
+      </c>
+      <c r="L151">
+        <v>1</v>
+      </c>
+      <c r="M151">
         <v>1</v>
       </c>
       <c r="T151">
         <v>0.5</v>
+      </c>
+      <c r="U151">
+        <v>1</v>
+      </c>
+      <c r="V151">
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:22" x14ac:dyDescent="0.3">
@@ -7246,6 +7285,7 @@
         <v>26</v>
       </c>
       <c r="C152">
+        <f t="shared" si="0"/>
         <v>151</v>
       </c>
       <c r="D152" s="6">
@@ -7258,31 +7298,31 @@
         <v>43678</v>
       </c>
       <c r="G152" s="6">
-        <v>43923</v>
+        <v>44104</v>
       </c>
       <c r="H152" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I152" s="1">
-        <v>43921</v>
+        <v>44104</v>
       </c>
       <c r="J152" s="5"/>
-      <c r="K152">
-        <v>1</v>
-      </c>
-      <c r="L152">
-        <v>1</v>
-      </c>
-      <c r="M152">
-        <v>1</v>
-      </c>
-      <c r="T152">
-        <v>0.5</v>
-      </c>
-      <c r="U152">
-        <v>1</v>
-      </c>
-      <c r="V152">
+      <c r="N152">
+        <v>1</v>
+      </c>
+      <c r="O152">
+        <v>1</v>
+      </c>
+      <c r="P152">
+        <v>1</v>
+      </c>
+      <c r="Q152">
+        <v>1</v>
+      </c>
+      <c r="R152">
+        <v>1</v>
+      </c>
+      <c r="S152">
         <v>1</v>
       </c>
     </row>
@@ -7294,6 +7334,7 @@
         <v>26</v>
       </c>
       <c r="C153">
+        <f t="shared" si="0"/>
         <v>152</v>
       </c>
       <c r="D153" s="6">
@@ -7306,31 +7347,31 @@
         <v>43678</v>
       </c>
       <c r="G153" s="6">
-        <v>44104</v>
+        <v>44265</v>
       </c>
       <c r="H153" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="I153" s="1">
-        <v>44104</v>
+        <v>44270</v>
       </c>
       <c r="J153" s="5"/>
-      <c r="N153">
-        <v>1</v>
-      </c>
-      <c r="O153">
-        <v>1</v>
-      </c>
-      <c r="P153">
-        <v>1</v>
-      </c>
-      <c r="Q153">
-        <v>1</v>
-      </c>
-      <c r="R153">
-        <v>1</v>
-      </c>
-      <c r="S153">
+      <c r="K153">
+        <v>1</v>
+      </c>
+      <c r="L153">
+        <v>1</v>
+      </c>
+      <c r="M153">
+        <v>0.5</v>
+      </c>
+      <c r="T153">
+        <v>1</v>
+      </c>
+      <c r="U153">
+        <v>1</v>
+      </c>
+      <c r="V153">
         <v>1</v>
       </c>
     </row>
@@ -7342,6 +7383,7 @@
         <v>26</v>
       </c>
       <c r="C154">
+        <f t="shared" si="0"/>
         <v>153</v>
       </c>
       <c r="D154" s="6">
@@ -7354,7 +7396,7 @@
         <v>43678</v>
       </c>
       <c r="G154" s="6">
-        <v>44265</v>
+        <v>44266</v>
       </c>
       <c r="H154" t="s">
         <v>61</v>
@@ -7390,6 +7432,7 @@
         <v>26</v>
       </c>
       <c r="C155">
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="D155" s="6">
@@ -7402,31 +7445,34 @@
         <v>43678</v>
       </c>
       <c r="G155" s="6">
-        <v>44266</v>
+        <v>44475</v>
       </c>
       <c r="H155" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="I155" s="1">
-        <v>44270</v>
+        <v>44469</v>
       </c>
       <c r="J155" s="5"/>
-      <c r="K155">
-        <v>1</v>
-      </c>
-      <c r="L155">
-        <v>1</v>
-      </c>
       <c r="M155">
         <v>0.5</v>
       </c>
-      <c r="T155">
-        <v>1</v>
-      </c>
-      <c r="U155">
-        <v>1</v>
-      </c>
-      <c r="V155">
+      <c r="N155">
+        <v>1</v>
+      </c>
+      <c r="O155">
+        <v>1</v>
+      </c>
+      <c r="P155">
+        <v>1</v>
+      </c>
+      <c r="Q155">
+        <v>1</v>
+      </c>
+      <c r="R155">
+        <v>1</v>
+      </c>
+      <c r="S155">
         <v>1</v>
       </c>
     </row>
@@ -7438,6 +7484,7 @@
         <v>26</v>
       </c>
       <c r="C156">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
       <c r="D156" s="6">
@@ -7450,7 +7497,7 @@
         <v>43678</v>
       </c>
       <c r="G156" s="6">
-        <v>44475</v>
+        <v>44476</v>
       </c>
       <c r="H156" t="s">
         <v>39</v>
@@ -7489,6 +7536,7 @@
         <v>26</v>
       </c>
       <c r="C157">
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="D157" s="6">
@@ -7501,7 +7549,7 @@
         <v>43678</v>
       </c>
       <c r="G157" s="6">
-        <v>44476</v>
+        <v>44477</v>
       </c>
       <c r="H157" t="s">
         <v>39</v>
@@ -7540,6 +7588,7 @@
         <v>26</v>
       </c>
       <c r="C158">
+        <f t="shared" si="0"/>
         <v>157</v>
       </c>
       <c r="D158" s="6">
@@ -7552,7 +7601,7 @@
         <v>43678</v>
       </c>
       <c r="G158" s="6">
-        <v>44477</v>
+        <v>44478</v>
       </c>
       <c r="H158" t="s">
         <v>39</v>
@@ -7591,6 +7640,7 @@
         <v>26</v>
       </c>
       <c r="C159">
+        <f t="shared" si="0"/>
         <v>158</v>
       </c>
       <c r="D159" s="6">
@@ -7603,34 +7653,31 @@
         <v>43678</v>
       </c>
       <c r="G159" s="6">
-        <v>44478</v>
+        <v>44643</v>
       </c>
       <c r="H159" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I159" s="1">
-        <v>44469</v>
+        <v>44651</v>
       </c>
       <c r="J159" s="5"/>
+      <c r="K159">
+        <v>1</v>
+      </c>
+      <c r="L159">
+        <v>1</v>
+      </c>
       <c r="M159">
-        <v>0.5</v>
-      </c>
-      <c r="N159">
-        <v>1</v>
-      </c>
-      <c r="O159">
-        <v>1</v>
-      </c>
-      <c r="P159">
-        <v>1</v>
-      </c>
-      <c r="Q159">
-        <v>1</v>
-      </c>
-      <c r="R159">
-        <v>1</v>
-      </c>
-      <c r="S159">
+        <v>1</v>
+      </c>
+      <c r="T159">
+        <v>1</v>
+      </c>
+      <c r="U159">
+        <v>1</v>
+      </c>
+      <c r="V159">
         <v>1</v>
       </c>
     </row>
@@ -7642,6 +7689,7 @@
         <v>26</v>
       </c>
       <c r="C160">
+        <f t="shared" si="0"/>
         <v>159</v>
       </c>
       <c r="D160" s="6">
@@ -7650,11 +7698,11 @@
       <c r="E160" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F160" s="1">
+      <c r="F160" s="10">
         <v>43678</v>
       </c>
       <c r="G160" s="6">
-        <v>44643</v>
+        <v>44644</v>
       </c>
       <c r="H160" t="s">
         <v>33</v>
@@ -7683,105 +7731,92 @@
       </c>
     </row>
     <row r="161" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+      <c r="A161" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C161">
+      <c r="C161" s="13">
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="D161" s="6">
+      <c r="D161" s="7">
         <v>43686</v>
       </c>
-      <c r="E161" s="1" t="s">
+      <c r="E161" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F161" s="10">
+      <c r="F161" s="8">
         <v>43678</v>
       </c>
-      <c r="G161" s="6">
-        <v>44644</v>
-      </c>
-      <c r="H161" t="s">
+      <c r="G161" s="7">
+        <v>44648</v>
+      </c>
+      <c r="H161" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I161" s="1">
+      <c r="I161" s="3">
         <v>44651</v>
       </c>
-      <c r="J161" s="5"/>
-      <c r="K161">
-        <v>1</v>
-      </c>
-      <c r="L161">
-        <v>1</v>
-      </c>
-      <c r="M161">
-        <v>1</v>
-      </c>
-      <c r="T161">
-        <v>1</v>
-      </c>
-      <c r="U161">
-        <v>1</v>
-      </c>
-      <c r="V161">
+      <c r="J161" s="9"/>
+      <c r="K161" s="2">
+        <v>1</v>
+      </c>
+      <c r="L161" s="2">
+        <v>1</v>
+      </c>
+      <c r="M161" s="2">
+        <v>1</v>
+      </c>
+      <c r="N161" s="2"/>
+      <c r="O161" s="2"/>
+      <c r="P161" s="2"/>
+      <c r="Q161" s="2"/>
+      <c r="R161" s="2"/>
+      <c r="S161" s="2"/>
+      <c r="T161" s="2">
+        <v>1</v>
+      </c>
+      <c r="U161" s="2">
+        <v>1</v>
+      </c>
+      <c r="V161" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C162" s="2">
+      <c r="A162" t="s">
+        <v>27</v>
+      </c>
+      <c r="B162" t="s">
+        <v>28</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="0"/>
         <v>161</v>
       </c>
-      <c r="D162" s="7">
-        <v>43686</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F162" s="8">
-        <v>43678</v>
-      </c>
-      <c r="G162" s="7">
-        <v>44648</v>
-      </c>
-      <c r="H162" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I162" s="3">
-        <v>44651</v>
-      </c>
-      <c r="J162" s="9"/>
-      <c r="K162" s="2">
-        <v>1</v>
-      </c>
-      <c r="L162" s="2">
-        <v>1</v>
-      </c>
-      <c r="M162" s="2">
-        <v>1</v>
-      </c>
-      <c r="N162" s="2"/>
-      <c r="O162" s="2"/>
-      <c r="P162" s="2"/>
-      <c r="Q162" s="2"/>
-      <c r="R162" s="2"/>
-      <c r="S162" s="2"/>
-      <c r="T162" s="2">
-        <v>1</v>
-      </c>
-      <c r="U162" s="2">
-        <v>1</v>
-      </c>
-      <c r="V162" s="2">
-        <v>1</v>
+      <c r="D162" s="6">
+        <v>43390</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F162" s="1">
+        <v>43388</v>
+      </c>
+      <c r="G162" s="6">
+        <v>43406</v>
+      </c>
+      <c r="H162" t="s">
+        <v>40</v>
+      </c>
+      <c r="I162" s="1">
+        <v>43404</v>
+      </c>
+      <c r="J162" s="5"/>
+      <c r="T162">
+        <v>0.5</v>
       </c>
     </row>
     <row r="163" spans="1:22" x14ac:dyDescent="0.3">
@@ -7792,6 +7827,7 @@
         <v>28</v>
       </c>
       <c r="C163">
+        <f t="shared" si="0"/>
         <v>162</v>
       </c>
       <c r="D163" s="6">
@@ -7804,16 +7840,16 @@
         <v>43388</v>
       </c>
       <c r="G163" s="6">
-        <v>43406</v>
+        <v>43420</v>
       </c>
       <c r="H163" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="I163" s="1">
-        <v>43404</v>
+        <v>43419</v>
       </c>
       <c r="J163" s="5"/>
-      <c r="T163">
+      <c r="U163">
         <v>0.5</v>
       </c>
     </row>
@@ -7825,6 +7861,7 @@
         <v>28</v>
       </c>
       <c r="C164">
+        <f t="shared" si="0"/>
         <v>163</v>
       </c>
       <c r="D164" s="6">
@@ -7837,16 +7874,19 @@
         <v>43388</v>
       </c>
       <c r="G164" s="6">
-        <v>43420</v>
+        <v>43445</v>
       </c>
       <c r="H164" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I164" s="1">
-        <v>43419</v>
+        <v>43449</v>
       </c>
       <c r="J164" s="5"/>
       <c r="U164">
+        <v>0.5</v>
+      </c>
+      <c r="V164">
         <v>0.5</v>
       </c>
     </row>
@@ -7858,6 +7898,7 @@
         <v>28</v>
       </c>
       <c r="C165">
+        <f t="shared" si="0"/>
         <v>164</v>
       </c>
       <c r="D165" s="6">
@@ -7870,17 +7911,23 @@
         <v>43388</v>
       </c>
       <c r="G165" s="6">
-        <v>43445</v>
+        <v>43546</v>
       </c>
       <c r="H165" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="I165" s="1">
-        <v>43449</v>
+        <v>43555</v>
       </c>
       <c r="J165" s="5"/>
-      <c r="U165">
-        <v>0.5</v>
+      <c r="K165">
+        <v>1</v>
+      </c>
+      <c r="L165">
+        <v>1</v>
+      </c>
+      <c r="M165">
+        <v>1</v>
       </c>
       <c r="V165">
         <v>0.5</v>
@@ -7894,6 +7941,7 @@
         <v>28</v>
       </c>
       <c r="C166">
+        <f t="shared" si="0"/>
         <v>165</v>
       </c>
       <c r="D166" s="6">
@@ -7906,7 +7954,7 @@
         <v>43388</v>
       </c>
       <c r="G166" s="6">
-        <v>43546</v>
+        <v>43560</v>
       </c>
       <c r="H166" t="s">
         <v>33</v>
@@ -7915,18 +7963,6 @@
         <v>43555</v>
       </c>
       <c r="J166" s="5"/>
-      <c r="K166">
-        <v>1</v>
-      </c>
-      <c r="L166">
-        <v>1</v>
-      </c>
-      <c r="M166">
-        <v>1</v>
-      </c>
-      <c r="V166">
-        <v>0.5</v>
-      </c>
     </row>
     <row r="167" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
@@ -7936,6 +7972,7 @@
         <v>28</v>
       </c>
       <c r="C167">
+        <f t="shared" si="0"/>
         <v>166</v>
       </c>
       <c r="D167" s="6">
@@ -7948,15 +7985,18 @@
         <v>43388</v>
       </c>
       <c r="G167" s="6">
-        <v>43560</v>
+        <v>43580</v>
       </c>
       <c r="H167" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I167" s="1">
-        <v>43555</v>
+        <v>43585</v>
       </c>
       <c r="J167" s="5"/>
+      <c r="N167">
+        <v>1</v>
+      </c>
     </row>
     <row r="168" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
@@ -7966,6 +8006,7 @@
         <v>28</v>
       </c>
       <c r="C168">
+        <f t="shared" si="0"/>
         <v>167</v>
       </c>
       <c r="D168" s="6">
@@ -7978,17 +8019,17 @@
         <v>43388</v>
       </c>
       <c r="G168" s="6">
-        <v>43580</v>
+        <v>43602</v>
       </c>
       <c r="H168" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="I168" s="1">
-        <v>43585</v>
+        <v>43600</v>
       </c>
       <c r="J168" s="5"/>
-      <c r="N168">
-        <v>1</v>
+      <c r="O168">
+        <v>0.5</v>
       </c>
     </row>
     <row r="169" spans="1:22" x14ac:dyDescent="0.3">
@@ -7999,6 +8040,7 @@
         <v>28</v>
       </c>
       <c r="C169">
+        <f t="shared" si="0"/>
         <v>168</v>
       </c>
       <c r="D169" s="6">
@@ -8011,16 +8053,19 @@
         <v>43388</v>
       </c>
       <c r="G169" s="6">
-        <v>43602</v>
+        <v>43629</v>
       </c>
       <c r="H169" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I169" s="1">
-        <v>43600</v>
+        <v>43631</v>
       </c>
       <c r="J169" s="5"/>
       <c r="O169">
+        <v>0.5</v>
+      </c>
+      <c r="P169">
         <v>0.5</v>
       </c>
     </row>
@@ -8032,6 +8077,7 @@
         <v>28</v>
       </c>
       <c r="C170">
+        <f t="shared" si="0"/>
         <v>169</v>
       </c>
       <c r="D170" s="6">
@@ -8044,119 +8090,118 @@
         <v>43388</v>
       </c>
       <c r="G170" s="6">
-        <v>43629</v>
+        <v>43670</v>
       </c>
       <c r="H170" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="I170" s="1">
-        <v>43631</v>
+        <v>43677</v>
       </c>
       <c r="J170" s="5"/>
-      <c r="O170">
-        <v>0.5</v>
-      </c>
       <c r="P170">
         <v>0.5</v>
       </c>
+      <c r="Q170">
+        <v>1</v>
+      </c>
     </row>
     <row r="171" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+      <c r="A171" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C171">
+      <c r="C171" s="13">
+        <f t="shared" si="0"/>
         <v>170</v>
       </c>
-      <c r="D171" s="6">
+      <c r="D171" s="7">
         <v>43390</v>
       </c>
-      <c r="E171" s="1" t="s">
+      <c r="E171" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F171" s="1">
+      <c r="F171" s="8">
         <v>43388</v>
       </c>
-      <c r="G171" s="6">
-        <v>43670</v>
-      </c>
-      <c r="H171" t="s">
-        <v>37</v>
-      </c>
-      <c r="I171" s="1">
-        <v>43677</v>
-      </c>
-      <c r="J171" s="5"/>
-      <c r="P171">
-        <v>0.5</v>
-      </c>
-      <c r="Q171">
+      <c r="G171" s="7">
+        <v>44375</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I171" s="3">
+        <v>44377</v>
+      </c>
+      <c r="J171" s="9"/>
+      <c r="K171" s="2">
+        <v>1</v>
+      </c>
+      <c r="L171" s="2">
+        <v>1</v>
+      </c>
+      <c r="M171" s="2">
+        <v>1</v>
+      </c>
+      <c r="N171" s="2">
+        <v>1</v>
+      </c>
+      <c r="O171" s="2">
+        <v>1</v>
+      </c>
+      <c r="P171" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q171" s="2"/>
+      <c r="R171" s="2">
+        <v>1</v>
+      </c>
+      <c r="S171" s="2">
+        <v>1</v>
+      </c>
+      <c r="T171" s="2">
+        <v>1</v>
+      </c>
+      <c r="U171" s="2">
+        <v>1</v>
+      </c>
+      <c r="V171" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A172" s="2" t="s">
+      <c r="A172" t="s">
         <v>27</v>
       </c>
-      <c r="B172" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C172" s="2">
+      <c r="B172" t="s">
+        <v>29</v>
+      </c>
+      <c r="C172">
+        <f t="shared" si="0"/>
         <v>171</v>
       </c>
-      <c r="D172" s="7">
-        <v>43390</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F172" s="8">
-        <v>43388</v>
-      </c>
-      <c r="G172" s="7">
-        <v>44375</v>
-      </c>
-      <c r="H172" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I172" s="3">
-        <v>44377</v>
-      </c>
-      <c r="J172" s="9"/>
-      <c r="K172" s="2">
-        <v>1</v>
-      </c>
-      <c r="L172" s="2">
-        <v>1</v>
-      </c>
-      <c r="M172" s="2">
-        <v>1</v>
-      </c>
-      <c r="N172" s="2">
-        <v>1</v>
-      </c>
-      <c r="O172" s="2">
-        <v>1</v>
-      </c>
-      <c r="P172" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q172" s="2"/>
-      <c r="R172" s="2">
-        <v>1</v>
-      </c>
-      <c r="S172" s="2">
-        <v>1</v>
-      </c>
-      <c r="T172" s="2">
-        <v>1</v>
-      </c>
-      <c r="U172" s="2">
-        <v>1</v>
-      </c>
-      <c r="V172" s="2">
+      <c r="D172" s="6">
+        <v>43404</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F172" s="1">
+        <v>43405</v>
+      </c>
+      <c r="G172" s="6">
+        <v>43431</v>
+      </c>
+      <c r="H172" t="s">
+        <v>41</v>
+      </c>
+      <c r="I172" s="1">
+        <v>43434</v>
+      </c>
+      <c r="J172" s="5"/>
+      <c r="U172">
         <v>1</v>
       </c>
     </row>
@@ -8168,6 +8213,7 @@
         <v>29</v>
       </c>
       <c r="C173">
+        <f t="shared" si="0"/>
         <v>172</v>
       </c>
       <c r="D173" s="6">
@@ -8180,17 +8226,17 @@
         <v>43405</v>
       </c>
       <c r="G173" s="6">
-        <v>43431</v>
+        <v>43446</v>
       </c>
       <c r="H173" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="I173" s="1">
-        <v>43434</v>
+        <v>43449</v>
       </c>
       <c r="J173" s="5"/>
-      <c r="U173">
-        <v>1</v>
+      <c r="V173">
+        <v>0.5</v>
       </c>
     </row>
     <row r="174" spans="1:22" x14ac:dyDescent="0.3">
@@ -8201,6 +8247,7 @@
         <v>29</v>
       </c>
       <c r="C174">
+        <f t="shared" si="0"/>
         <v>173</v>
       </c>
       <c r="D174" s="6">
@@ -8213,15 +8260,24 @@
         <v>43405</v>
       </c>
       <c r="G174" s="6">
-        <v>43446</v>
+        <v>43553</v>
       </c>
       <c r="H174" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="I174" s="1">
-        <v>43449</v>
+        <v>43555</v>
       </c>
       <c r="J174" s="5"/>
+      <c r="K174">
+        <v>1</v>
+      </c>
+      <c r="L174">
+        <v>1</v>
+      </c>
+      <c r="M174">
+        <v>1</v>
+      </c>
       <c r="V174">
         <v>0.5</v>
       </c>
@@ -8234,6 +8290,7 @@
         <v>29</v>
       </c>
       <c r="C175">
+        <f t="shared" si="0"/>
         <v>174</v>
       </c>
       <c r="D175" s="6">
@@ -8246,25 +8303,16 @@
         <v>43405</v>
       </c>
       <c r="G175" s="6">
-        <v>43553</v>
+        <v>43574</v>
       </c>
       <c r="H175" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I175" s="1">
-        <v>43555</v>
+        <v>43570</v>
       </c>
       <c r="J175" s="5"/>
-      <c r="K175">
-        <v>1</v>
-      </c>
-      <c r="L175">
-        <v>1</v>
-      </c>
-      <c r="M175">
-        <v>1</v>
-      </c>
-      <c r="V175">
+      <c r="N175">
         <v>0.5</v>
       </c>
     </row>
@@ -8276,6 +8324,7 @@
         <v>29</v>
       </c>
       <c r="C176">
+        <f t="shared" si="0"/>
         <v>175</v>
       </c>
       <c r="D176" s="6">
@@ -8288,13 +8337,13 @@
         <v>43405</v>
       </c>
       <c r="G176" s="6">
-        <v>43574</v>
+        <v>43594</v>
       </c>
       <c r="H176" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="I176" s="1">
-        <v>43570</v>
+        <v>43585</v>
       </c>
       <c r="J176" s="5"/>
       <c r="N176">
@@ -8309,6 +8358,7 @@
         <v>29</v>
       </c>
       <c r="C177">
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
       <c r="D177" s="6">
@@ -8321,17 +8371,17 @@
         <v>43405</v>
       </c>
       <c r="G177" s="6">
-        <v>43594</v>
+        <v>43613</v>
       </c>
       <c r="H177" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I177" s="1">
-        <v>43585</v>
+        <v>43616</v>
       </c>
       <c r="J177" s="5"/>
-      <c r="N177">
-        <v>0.5</v>
+      <c r="O177">
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:22" x14ac:dyDescent="0.3">
@@ -8342,6 +8392,7 @@
         <v>29</v>
       </c>
       <c r="C178">
+        <f t="shared" si="0"/>
         <v>177</v>
       </c>
       <c r="D178" s="6">
@@ -8354,16 +8405,16 @@
         <v>43405</v>
       </c>
       <c r="G178" s="6">
-        <v>43613</v>
+        <v>43647</v>
       </c>
       <c r="H178" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I178" s="1">
-        <v>43616</v>
+        <v>43646</v>
       </c>
       <c r="J178" s="5"/>
-      <c r="O178">
+      <c r="P178">
         <v>1</v>
       </c>
     </row>
@@ -8375,6 +8426,7 @@
         <v>29</v>
       </c>
       <c r="C179">
+        <f t="shared" si="0"/>
         <v>178</v>
       </c>
       <c r="D179" s="6">
@@ -8387,116 +8439,118 @@
         <v>43405</v>
       </c>
       <c r="G179" s="6">
-        <v>43647</v>
+        <v>43684</v>
       </c>
       <c r="H179" t="s">
+        <v>37</v>
+      </c>
+      <c r="I179" s="1">
+        <v>43677</v>
+      </c>
+      <c r="J179" s="5"/>
+      <c r="Q179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A180" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C180" s="13">
+        <f t="shared" si="0"/>
+        <v>179</v>
+      </c>
+      <c r="D180" s="7">
+        <v>43404</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F180" s="8">
+        <v>43405</v>
+      </c>
+      <c r="G180" s="7">
+        <v>44376</v>
+      </c>
+      <c r="H180" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I179" s="1">
-        <v>43646</v>
-      </c>
-      <c r="J179" s="5"/>
-      <c r="P179">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="180" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
+      <c r="I180" s="3">
+        <v>44377</v>
+      </c>
+      <c r="J180" s="9">
+        <v>1</v>
+      </c>
+      <c r="K180" s="2">
+        <v>1</v>
+      </c>
+      <c r="L180" s="2">
+        <v>1</v>
+      </c>
+      <c r="M180" s="2">
+        <v>1</v>
+      </c>
+      <c r="N180" s="2">
+        <v>1</v>
+      </c>
+      <c r="O180" s="2">
+        <v>1</v>
+      </c>
+      <c r="P180" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q180" s="2"/>
+      <c r="R180" s="2">
+        <v>1</v>
+      </c>
+      <c r="S180" s="2">
+        <v>1</v>
+      </c>
+      <c r="T180" s="2">
+        <v>1</v>
+      </c>
+      <c r="U180" s="2">
+        <v>1</v>
+      </c>
+      <c r="V180" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A181" t="s">
         <v>27</v>
       </c>
-      <c r="B180" t="s">
-        <v>29</v>
-      </c>
-      <c r="C180">
-        <v>179</v>
-      </c>
-      <c r="D180" s="6">
-        <v>43404</v>
-      </c>
-      <c r="E180" s="1" t="s">
+      <c r="B181" t="s">
+        <v>30</v>
+      </c>
+      <c r="C181">
+        <f t="shared" ref="C181:C188" si="1">C180+1</f>
+        <v>180</v>
+      </c>
+      <c r="D181" s="6">
+        <v>43402</v>
+      </c>
+      <c r="E181" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F180" s="1">
+      <c r="F181" s="1">
         <v>43405</v>
       </c>
-      <c r="G180" s="6">
-        <v>43684</v>
-      </c>
-      <c r="H180" t="s">
-        <v>37</v>
-      </c>
-      <c r="I180" s="1">
-        <v>43677</v>
-      </c>
-      <c r="J180" s="5"/>
-      <c r="Q180">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="181" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A181" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B181" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C181" s="2">
-        <v>180</v>
-      </c>
-      <c r="D181" s="7">
-        <v>43404</v>
-      </c>
-      <c r="E181" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F181" s="8">
-        <v>43405</v>
-      </c>
-      <c r="G181" s="7">
-        <v>44376</v>
-      </c>
-      <c r="H181" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I181" s="3">
-        <v>44377</v>
-      </c>
-      <c r="J181" s="9">
-        <v>1</v>
-      </c>
-      <c r="K181" s="2">
-        <v>1</v>
-      </c>
-      <c r="L181" s="2">
-        <v>1</v>
-      </c>
-      <c r="M181" s="2">
-        <v>1</v>
-      </c>
-      <c r="N181" s="2">
-        <v>1</v>
-      </c>
-      <c r="O181" s="2">
-        <v>1</v>
-      </c>
-      <c r="P181" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q181" s="2"/>
-      <c r="R181" s="2">
-        <v>1</v>
-      </c>
-      <c r="S181" s="2">
-        <v>1</v>
-      </c>
-      <c r="T181" s="2">
-        <v>1</v>
-      </c>
-      <c r="U181" s="2">
-        <v>1</v>
-      </c>
-      <c r="V181" s="2">
-        <v>1</v>
+      <c r="G181" s="6">
+        <v>43420</v>
+      </c>
+      <c r="H181" t="s">
+        <v>67</v>
+      </c>
+      <c r="I181" s="1">
+        <v>43419</v>
+      </c>
+      <c r="J181" s="5"/>
+      <c r="U181">
+        <v>0.5</v>
       </c>
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.3">
@@ -8507,6 +8561,7 @@
         <v>30</v>
       </c>
       <c r="C182">
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="D182" s="6">
@@ -8519,13 +8574,13 @@
         <v>43405</v>
       </c>
       <c r="G182" s="6">
-        <v>43420</v>
+        <v>43432</v>
       </c>
       <c r="H182" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="I182" s="1">
-        <v>43419</v>
+        <v>43434</v>
       </c>
       <c r="J182" s="5"/>
       <c r="U182">
@@ -8540,6 +8595,7 @@
         <v>30</v>
       </c>
       <c r="C183">
+        <f t="shared" si="1"/>
         <v>182</v>
       </c>
       <c r="D183" s="6">
@@ -8552,17 +8608,29 @@
         <v>43405</v>
       </c>
       <c r="G183" s="6">
-        <v>43432</v>
+        <v>43581</v>
       </c>
       <c r="H183" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I183" s="1">
-        <v>43434</v>
+        <v>43585</v>
       </c>
       <c r="J183" s="5"/>
-      <c r="U183">
-        <v>0.5</v>
+      <c r="K183">
+        <v>1</v>
+      </c>
+      <c r="L183">
+        <v>1</v>
+      </c>
+      <c r="M183">
+        <v>1</v>
+      </c>
+      <c r="N183">
+        <v>1</v>
+      </c>
+      <c r="V183">
+        <v>1</v>
       </c>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.3">
@@ -8573,6 +8641,7 @@
         <v>30</v>
       </c>
       <c r="C184">
+        <f t="shared" si="1"/>
         <v>183</v>
       </c>
       <c r="D184" s="6">
@@ -8585,29 +8654,17 @@
         <v>43405</v>
       </c>
       <c r="G184" s="6">
-        <v>43581</v>
+        <v>43601</v>
       </c>
       <c r="H184" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="I184" s="1">
-        <v>43585</v>
+        <v>43600</v>
       </c>
       <c r="J184" s="5"/>
-      <c r="K184">
-        <v>1</v>
-      </c>
-      <c r="L184">
-        <v>1</v>
-      </c>
-      <c r="M184">
-        <v>1</v>
-      </c>
-      <c r="N184">
-        <v>1</v>
-      </c>
-      <c r="V184">
-        <v>1</v>
+      <c r="O184">
+        <v>0.5</v>
       </c>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.3">
@@ -8618,6 +8675,7 @@
         <v>30</v>
       </c>
       <c r="C185">
+        <f t="shared" si="1"/>
         <v>184</v>
       </c>
       <c r="D185" s="6">
@@ -8630,13 +8688,13 @@
         <v>43405</v>
       </c>
       <c r="G185" s="6">
-        <v>43601</v>
+        <v>43614</v>
       </c>
       <c r="H185" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="I185" s="1">
-        <v>43600</v>
+        <v>43616</v>
       </c>
       <c r="J185" s="5"/>
       <c r="O185">
@@ -8651,6 +8709,7 @@
         <v>30</v>
       </c>
       <c r="C186">
+        <f t="shared" si="1"/>
         <v>185</v>
       </c>
       <c r="D186" s="6">
@@ -8663,17 +8722,17 @@
         <v>43405</v>
       </c>
       <c r="G186" s="6">
-        <v>43614</v>
+        <v>43648</v>
       </c>
       <c r="H186" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I186" s="1">
-        <v>43616</v>
+        <v>43646</v>
       </c>
       <c r="J186" s="5"/>
-      <c r="O186">
-        <v>0.5</v>
+      <c r="P186">
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.3">
@@ -8684,6 +8743,7 @@
         <v>30</v>
       </c>
       <c r="C187">
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="D187" s="6">
@@ -8696,115 +8756,83 @@
         <v>43405</v>
       </c>
       <c r="G187" s="6">
-        <v>43648</v>
+        <v>43683</v>
       </c>
       <c r="H187" t="s">
+        <v>37</v>
+      </c>
+      <c r="I187" s="1">
+        <v>43677</v>
+      </c>
+      <c r="J187" s="5"/>
+      <c r="Q187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A188" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C188" s="13">
+        <f t="shared" si="1"/>
+        <v>187</v>
+      </c>
+      <c r="D188" s="7">
+        <v>43402</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F188" s="8">
+        <v>43405</v>
+      </c>
+      <c r="G188" s="7">
+        <v>44376</v>
+      </c>
+      <c r="H188" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I187" s="1">
-        <v>43646</v>
-      </c>
-      <c r="J187" s="5"/>
-      <c r="P187">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="188" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
-        <v>27</v>
-      </c>
-      <c r="B188" t="s">
-        <v>30</v>
-      </c>
-      <c r="C188">
-        <v>187</v>
-      </c>
-      <c r="D188" s="6">
-        <v>43402</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F188" s="1">
-        <v>43405</v>
-      </c>
-      <c r="G188" s="6">
-        <v>43683</v>
-      </c>
-      <c r="H188" t="s">
-        <v>37</v>
-      </c>
-      <c r="I188" s="1">
-        <v>43677</v>
-      </c>
-      <c r="J188" s="5"/>
-      <c r="Q188">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A189" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C189" s="2">
-        <v>188</v>
-      </c>
-      <c r="D189" s="7">
-        <v>43402</v>
-      </c>
-      <c r="E189" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F189" s="8">
-        <v>43405</v>
-      </c>
-      <c r="G189" s="7">
-        <v>44376</v>
-      </c>
-      <c r="H189" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I189" s="3">
+      <c r="I188" s="3">
         <v>44377</v>
       </c>
-      <c r="J189" s="9">
-        <v>1</v>
-      </c>
-      <c r="K189" s="2">
-        <v>1</v>
-      </c>
-      <c r="L189" s="2">
-        <v>1</v>
-      </c>
-      <c r="M189" s="2">
-        <v>1</v>
-      </c>
-      <c r="N189" s="2">
-        <v>1</v>
-      </c>
-      <c r="O189" s="2">
-        <v>1</v>
-      </c>
-      <c r="P189" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q189" s="2"/>
-      <c r="R189" s="2">
-        <v>1</v>
-      </c>
-      <c r="S189" s="2">
-        <v>1</v>
-      </c>
-      <c r="T189" s="2">
-        <v>1</v>
-      </c>
-      <c r="U189" s="2">
-        <v>1</v>
-      </c>
-      <c r="V189" s="2">
+      <c r="J188" s="9">
+        <v>1</v>
+      </c>
+      <c r="K188" s="2">
+        <v>1</v>
+      </c>
+      <c r="L188" s="2">
+        <v>1</v>
+      </c>
+      <c r="M188" s="2">
+        <v>1</v>
+      </c>
+      <c r="N188" s="2">
+        <v>1</v>
+      </c>
+      <c r="O188" s="2">
+        <v>1</v>
+      </c>
+      <c r="P188" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q188" s="2"/>
+      <c r="R188" s="2">
+        <v>1</v>
+      </c>
+      <c r="S188" s="2">
+        <v>1</v>
+      </c>
+      <c r="T188" s="2">
+        <v>1</v>
+      </c>
+      <c r="U188" s="2">
+        <v>1</v>
+      </c>
+      <c r="V188" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
I forgot there was another tab on the Excel spreadsheet whose SiteDateID also needed to be changed lol
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.3_months-to-include-for-precip-normals-comparison.xlsx
+++ b/data/data-wrangling-intermediate/03.3_months-to-include-for-precip-normals-comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/data-wrangling-intermediate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3397" documentId="8_{89B2EEDE-D508-4F25-B24C-4C204CBA613B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28678E8F-E229-4CFF-89C4-8ECE709DAF0F}"/>
+  <xr:revisionPtr revIDLastSave="3401" documentId="8_{89B2EEDE-D508-4F25-B24C-4C204CBA613B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{23184C8A-1C92-4784-AF62-2714E7846ECB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{1028A4EE-DCCB-47E3-9760-4B4BA3E1195B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{1028A4EE-DCCB-47E3-9760-4B4BA3E1195B}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="3" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1565" uniqueCount="76">
   <si>
     <t>Region</t>
   </si>
@@ -1034,7 +1034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314917C4-A3F7-4522-885F-2395A80BBF8D}">
   <dimension ref="A1:V188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C188" activeCellId="10" sqref="C115 C120 C126 C131 C136 C140 C149 C161 C171 C180 C188"/>
     </sheetView>
@@ -8845,11 +8845,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F311CDD9-2A96-4278-89CD-C73D448DA6CC}">
-  <dimension ref="A1:V189"/>
+  <dimension ref="A1:V188"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C188" activeCellId="9" sqref="C120 C126 C131 C136 C140 C149 C161 C171 C180 C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14052,52 +14052,41 @@
       </c>
     </row>
     <row r="116" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
+      <c r="A116" t="s">
         <v>16</v>
       </c>
-      <c r="B116" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C116" s="2">
+      <c r="B116" t="s">
+        <v>18</v>
+      </c>
+      <c r="C116">
+        <f>C115+1</f>
         <v>115</v>
       </c>
-      <c r="D116" s="7">
-        <v>43903</v>
-      </c>
-      <c r="E116" s="3" t="s">
+      <c r="D116" s="6">
+        <v>43907</v>
+      </c>
+      <c r="E116" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="F116" s="8">
+      <c r="F116" s="1">
         <v>43905</v>
       </c>
-      <c r="G116" s="7">
-        <v>44666</v>
-      </c>
-      <c r="H116" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I116" s="3">
-        <v>44666</v>
-      </c>
-      <c r="J116" s="9">
-        <v>2</v>
-      </c>
-      <c r="K116" s="2"/>
-      <c r="L116" s="2"/>
-      <c r="M116" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N116" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O116" s="2"/>
-      <c r="P116" s="2"/>
-      <c r="Q116" s="2"/>
-      <c r="R116" s="2"/>
-      <c r="S116" s="2"/>
-      <c r="T116" s="2"/>
-      <c r="U116" s="2"/>
-      <c r="V116" s="2"/>
+      <c r="G116" s="6">
+        <v>43951</v>
+      </c>
+      <c r="H116" t="s">
+        <v>34</v>
+      </c>
+      <c r="I116" s="1">
+        <v>43951</v>
+      </c>
+      <c r="J116" s="5"/>
+      <c r="M116">
+        <v>0.5</v>
+      </c>
+      <c r="N116">
+        <v>1</v>
+      </c>
     </row>
     <row r="117" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
@@ -14107,6 +14096,7 @@
         <v>18</v>
       </c>
       <c r="C117">
+        <f t="shared" ref="C117:C180" si="0">C116+1</f>
         <v>116</v>
       </c>
       <c r="D117" s="6">
@@ -14119,20 +14109,19 @@
         <v>43905</v>
       </c>
       <c r="G117" s="6">
-        <v>43951</v>
+        <v>44292</v>
       </c>
       <c r="H117" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I117" s="1">
-        <v>43951</v>
-      </c>
-      <c r="J117" s="5"/>
+        <v>44286</v>
+      </c>
+      <c r="J117" s="5">
+        <v>1</v>
+      </c>
       <c r="M117">
         <v>0.5</v>
-      </c>
-      <c r="N117">
-        <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:22" x14ac:dyDescent="0.3">
@@ -14143,30 +14132,38 @@
         <v>18</v>
       </c>
       <c r="C118">
+        <f t="shared" si="0"/>
         <v>117</v>
       </c>
       <c r="D118" s="6">
-        <v>43907</v>
+        <v>44578</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F118" s="1">
-        <v>43905</v>
+        <v>44576</v>
       </c>
       <c r="G118" s="6">
-        <v>44292</v>
+        <v>44664</v>
       </c>
       <c r="H118" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I118" s="1">
-        <v>44286</v>
-      </c>
-      <c r="J118" s="5">
+        <v>44666</v>
+      </c>
+      <c r="J118" s="5"/>
+      <c r="K118">
+        <v>0.5</v>
+      </c>
+      <c r="L118">
         <v>1</v>
       </c>
       <c r="M118">
+        <v>1</v>
+      </c>
+      <c r="N118">
         <v>0.5</v>
       </c>
     </row>
@@ -14178,10 +14175,11 @@
         <v>18</v>
       </c>
       <c r="C119">
+        <f t="shared" si="0"/>
         <v>118</v>
       </c>
       <c r="D119" s="6">
-        <v>44578</v>
+        <v>44576</v>
       </c>
       <c r="E119" s="1" t="s">
         <v>63</v>
@@ -14213,94 +14211,96 @@
       </c>
     </row>
     <row r="120" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+      <c r="A120" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="13">
+        <f t="shared" si="0"/>
         <v>119</v>
       </c>
-      <c r="D120" s="6">
-        <v>44576</v>
-      </c>
-      <c r="E120" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F120" s="1">
-        <v>44576</v>
-      </c>
-      <c r="G120" s="6">
+      <c r="D120" s="7">
+        <v>43907</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F120" s="8">
+        <v>43905</v>
+      </c>
+      <c r="G120" s="7">
         <v>44664</v>
       </c>
-      <c r="H120" t="s">
+      <c r="H120" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I120" s="1">
+      <c r="I120" s="3">
         <v>44666</v>
       </c>
-      <c r="J120" s="5"/>
-      <c r="K120">
-        <v>0.5</v>
-      </c>
-      <c r="L120">
-        <v>1</v>
-      </c>
-      <c r="M120">
-        <v>1</v>
-      </c>
-      <c r="N120">
-        <v>0.5</v>
-      </c>
+      <c r="J120" s="9">
+        <v>2</v>
+      </c>
+      <c r="K120" s="2"/>
+      <c r="L120" s="2"/>
+      <c r="M120" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="N120" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="O120" s="2"/>
+      <c r="P120" s="2"/>
+      <c r="Q120" s="2"/>
+      <c r="R120" s="2"/>
+      <c r="S120" s="2"/>
+      <c r="T120" s="2"/>
+      <c r="U120" s="2"/>
+      <c r="V120" s="2"/>
     </row>
     <row r="121" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C121" s="2">
+      <c r="A121" t="s">
+        <v>19</v>
+      </c>
+      <c r="B121" t="s">
+        <v>20</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="D121" s="7">
-        <v>43907</v>
-      </c>
-      <c r="E121" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F121" s="8">
-        <v>43905</v>
-      </c>
-      <c r="G121" s="7">
-        <v>44664</v>
-      </c>
-      <c r="H121" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="I121" s="3">
-        <v>44666</v>
-      </c>
-      <c r="J121" s="9">
-        <v>2</v>
-      </c>
-      <c r="K121" s="2"/>
-      <c r="L121" s="2"/>
-      <c r="M121" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="N121" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="O121" s="2"/>
-      <c r="P121" s="2"/>
-      <c r="Q121" s="2"/>
-      <c r="R121" s="2"/>
-      <c r="S121" s="2"/>
-      <c r="T121" s="2"/>
-      <c r="U121" s="2"/>
-      <c r="V121" s="2"/>
+      <c r="D121" s="6">
+        <v>43818</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F121" s="1">
+        <v>43814</v>
+      </c>
+      <c r="G121" s="6">
+        <v>43920</v>
+      </c>
+      <c r="H121" t="s">
+        <v>33</v>
+      </c>
+      <c r="I121" s="1">
+        <v>43920</v>
+      </c>
+      <c r="J121" s="5"/>
+      <c r="K121">
+        <v>1</v>
+      </c>
+      <c r="L121">
+        <v>1</v>
+      </c>
+      <c r="M121">
+        <v>1</v>
+      </c>
+      <c r="V121">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="122" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
@@ -14310,6 +14310,7 @@
         <v>20</v>
       </c>
       <c r="C122">
+        <f t="shared" si="0"/>
         <v>121</v>
       </c>
       <c r="D122" s="6">
@@ -14322,13 +14323,13 @@
         <v>43814</v>
       </c>
       <c r="G122" s="6">
-        <v>43920</v>
+        <v>44118</v>
       </c>
       <c r="H122" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="I122" s="1">
-        <v>43920</v>
+        <v>44119</v>
       </c>
       <c r="J122" s="5"/>
       <c r="K122">
@@ -14339,6 +14340,27 @@
       </c>
       <c r="M122">
         <v>1</v>
+      </c>
+      <c r="N122">
+        <v>1</v>
+      </c>
+      <c r="O122">
+        <v>1</v>
+      </c>
+      <c r="P122">
+        <v>1</v>
+      </c>
+      <c r="Q122">
+        <v>1</v>
+      </c>
+      <c r="R122">
+        <v>1</v>
+      </c>
+      <c r="S122">
+        <v>1</v>
+      </c>
+      <c r="T122">
+        <v>0.5</v>
       </c>
       <c r="V122">
         <v>0.5</v>
@@ -14352,6 +14374,7 @@
         <v>20</v>
       </c>
       <c r="C123">
+        <f t="shared" si="0"/>
         <v>122</v>
       </c>
       <c r="D123" s="6">
@@ -14364,15 +14387,17 @@
         <v>43814</v>
       </c>
       <c r="G123" s="6">
-        <v>44118</v>
+        <v>44288</v>
       </c>
       <c r="H123" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I123" s="1">
-        <v>44119</v>
-      </c>
-      <c r="J123" s="5"/>
+        <v>44286</v>
+      </c>
+      <c r="J123" s="5">
+        <v>1</v>
+      </c>
       <c r="K123">
         <v>1</v>
       </c>
@@ -14381,27 +14406,6 @@
       </c>
       <c r="M123">
         <v>1</v>
-      </c>
-      <c r="N123">
-        <v>1</v>
-      </c>
-      <c r="O123">
-        <v>1</v>
-      </c>
-      <c r="P123">
-        <v>1</v>
-      </c>
-      <c r="Q123">
-        <v>1</v>
-      </c>
-      <c r="R123">
-        <v>1</v>
-      </c>
-      <c r="S123">
-        <v>1</v>
-      </c>
-      <c r="T123">
-        <v>0.5</v>
       </c>
       <c r="V123">
         <v>0.5</v>
@@ -14415,6 +14419,7 @@
         <v>20</v>
       </c>
       <c r="C124">
+        <f t="shared" si="0"/>
         <v>123</v>
       </c>
       <c r="D124" s="6">
@@ -14427,13 +14432,13 @@
         <v>43814</v>
       </c>
       <c r="G124" s="6">
-        <v>44288</v>
+        <v>44473</v>
       </c>
       <c r="H124" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I124" s="1">
-        <v>44286</v>
+        <v>44469</v>
       </c>
       <c r="J124" s="5">
         <v>1</v>
@@ -14445,6 +14450,24 @@
         <v>1</v>
       </c>
       <c r="M124">
+        <v>1</v>
+      </c>
+      <c r="N124">
+        <v>1</v>
+      </c>
+      <c r="O124">
+        <v>1</v>
+      </c>
+      <c r="P124">
+        <v>1</v>
+      </c>
+      <c r="Q124">
+        <v>1</v>
+      </c>
+      <c r="R124">
+        <v>1</v>
+      </c>
+      <c r="S124">
         <v>1</v>
       </c>
       <c r="V124">
@@ -14459,6 +14482,7 @@
         <v>20</v>
       </c>
       <c r="C125">
+        <f t="shared" si="0"/>
         <v>124</v>
       </c>
       <c r="D125" s="6">
@@ -14471,16 +14495,16 @@
         <v>43814</v>
       </c>
       <c r="G125" s="6">
-        <v>44473</v>
+        <v>44649</v>
       </c>
       <c r="H125" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I125" s="1">
-        <v>44469</v>
+        <v>44651</v>
       </c>
       <c r="J125" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K125">
         <v>1</v>
@@ -14491,122 +14515,104 @@
       <c r="M125">
         <v>1</v>
       </c>
-      <c r="N125">
-        <v>1</v>
-      </c>
-      <c r="O125">
-        <v>1</v>
-      </c>
-      <c r="P125">
-        <v>1</v>
-      </c>
-      <c r="Q125">
-        <v>1</v>
-      </c>
-      <c r="R125">
-        <v>1</v>
-      </c>
-      <c r="S125">
-        <v>1</v>
-      </c>
       <c r="V125">
         <v>0.5</v>
       </c>
     </row>
     <row r="126" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+      <c r="A126" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="13">
+        <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="D126" s="6">
+      <c r="D126" s="7">
         <v>43818</v>
       </c>
-      <c r="E126" s="1" t="s">
+      <c r="E126" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F126" s="1">
+      <c r="F126" s="8">
         <v>43814</v>
       </c>
-      <c r="G126" s="6">
-        <v>44649</v>
-      </c>
-      <c r="H126" t="s">
+      <c r="G126" s="7">
+        <v>45009</v>
+      </c>
+      <c r="H126" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I126" s="1">
-        <v>44651</v>
-      </c>
-      <c r="J126" s="5">
-        <v>2</v>
-      </c>
-      <c r="K126">
-        <v>1</v>
-      </c>
-      <c r="L126">
-        <v>1</v>
-      </c>
-      <c r="M126">
-        <v>1</v>
-      </c>
-      <c r="V126">
+      <c r="I126" s="3">
+        <v>45016</v>
+      </c>
+      <c r="J126" s="9">
+        <v>3</v>
+      </c>
+      <c r="K126" s="2">
+        <v>1</v>
+      </c>
+      <c r="L126" s="2">
+        <v>1</v>
+      </c>
+      <c r="M126" s="2">
+        <v>1</v>
+      </c>
+      <c r="N126" s="2"/>
+      <c r="O126" s="2"/>
+      <c r="P126" s="2"/>
+      <c r="Q126" s="2"/>
+      <c r="R126" s="2"/>
+      <c r="S126" s="2"/>
+      <c r="T126" s="2"/>
+      <c r="U126" s="2"/>
+      <c r="V126" s="2">
         <v>0.5</v>
       </c>
     </row>
     <row r="127" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
+      <c r="A127" t="s">
         <v>19</v>
       </c>
-      <c r="B127" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C127" s="2">
+      <c r="B127" t="s">
+        <v>21</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="0"/>
         <v>126</v>
       </c>
-      <c r="D127" s="7">
-        <v>43818</v>
-      </c>
-      <c r="E127" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F127" s="8">
-        <v>43814</v>
-      </c>
-      <c r="G127" s="7">
-        <v>45009</v>
-      </c>
-      <c r="H127" s="2" t="s">
+      <c r="D127" s="6">
+        <v>43794</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F127" s="1">
+        <v>43800</v>
+      </c>
+      <c r="G127" s="6">
+        <v>43916</v>
+      </c>
+      <c r="H127" t="s">
         <v>33</v>
       </c>
-      <c r="I127" s="3">
-        <v>45016</v>
-      </c>
-      <c r="J127" s="9">
-        <v>3</v>
-      </c>
-      <c r="K127" s="2">
-        <v>1</v>
-      </c>
-      <c r="L127" s="2">
-        <v>1</v>
-      </c>
-      <c r="M127" s="2">
-        <v>1</v>
-      </c>
-      <c r="N127" s="2"/>
-      <c r="O127" s="2"/>
-      <c r="P127" s="2"/>
-      <c r="Q127" s="2"/>
-      <c r="R127" s="2"/>
-      <c r="S127" s="2"/>
-      <c r="T127" s="2"/>
-      <c r="U127" s="2"/>
-      <c r="V127" s="2">
-        <v>0.5</v>
+      <c r="I127" s="1">
+        <v>43920</v>
+      </c>
+      <c r="J127" s="5"/>
+      <c r="K127">
+        <v>1</v>
+      </c>
+      <c r="L127">
+        <v>1</v>
+      </c>
+      <c r="M127">
+        <v>1</v>
+      </c>
+      <c r="V127">
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:22" x14ac:dyDescent="0.3">
@@ -14617,6 +14623,7 @@
         <v>21</v>
       </c>
       <c r="C128">
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="D128" s="6">
@@ -14629,13 +14636,13 @@
         <v>43800</v>
       </c>
       <c r="G128" s="6">
-        <v>43916</v>
+        <v>44116</v>
       </c>
       <c r="H128" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="I128" s="1">
-        <v>43920</v>
+        <v>44119</v>
       </c>
       <c r="J128" s="5"/>
       <c r="K128">
@@ -14646,6 +14653,27 @@
       </c>
       <c r="M128">
         <v>1</v>
+      </c>
+      <c r="N128">
+        <v>1</v>
+      </c>
+      <c r="O128">
+        <v>1</v>
+      </c>
+      <c r="P128">
+        <v>1</v>
+      </c>
+      <c r="Q128">
+        <v>1</v>
+      </c>
+      <c r="R128">
+        <v>1</v>
+      </c>
+      <c r="S128">
+        <v>1</v>
+      </c>
+      <c r="T128">
+        <v>0.5</v>
       </c>
       <c r="V128">
         <v>1</v>
@@ -14659,6 +14687,7 @@
         <v>21</v>
       </c>
       <c r="C129">
+        <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="D129" s="6">
@@ -14671,15 +14700,17 @@
         <v>43800</v>
       </c>
       <c r="G129" s="6">
-        <v>44116</v>
+        <v>44285</v>
       </c>
       <c r="H129" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I129" s="1">
-        <v>44119</v>
-      </c>
-      <c r="J129" s="5"/>
+        <v>44286</v>
+      </c>
+      <c r="J129" s="5">
+        <v>1</v>
+      </c>
       <c r="K129">
         <v>1</v>
       </c>
@@ -14688,27 +14719,6 @@
       </c>
       <c r="M129">
         <v>1</v>
-      </c>
-      <c r="N129">
-        <v>1</v>
-      </c>
-      <c r="O129">
-        <v>1</v>
-      </c>
-      <c r="P129">
-        <v>1</v>
-      </c>
-      <c r="Q129">
-        <v>1</v>
-      </c>
-      <c r="R129">
-        <v>1</v>
-      </c>
-      <c r="S129">
-        <v>1</v>
-      </c>
-      <c r="T129">
-        <v>0.5</v>
       </c>
       <c r="V129">
         <v>1</v>
@@ -14722,6 +14732,7 @@
         <v>21</v>
       </c>
       <c r="C130">
+        <f t="shared" si="0"/>
         <v>129</v>
       </c>
       <c r="D130" s="6">
@@ -14734,141 +14745,141 @@
         <v>43800</v>
       </c>
       <c r="G130" s="6">
-        <v>44285</v>
+        <v>44475</v>
       </c>
       <c r="H130" t="s">
+        <v>39</v>
+      </c>
+      <c r="I130" s="1">
+        <v>44469</v>
+      </c>
+      <c r="J130" s="5">
+        <v>1</v>
+      </c>
+      <c r="K130">
+        <v>1</v>
+      </c>
+      <c r="L130">
+        <v>1</v>
+      </c>
+      <c r="M130">
+        <v>1</v>
+      </c>
+      <c r="N130">
+        <v>1</v>
+      </c>
+      <c r="O130">
+        <v>1</v>
+      </c>
+      <c r="P130">
+        <v>1</v>
+      </c>
+      <c r="Q130">
+        <v>1</v>
+      </c>
+      <c r="R130">
+        <v>1</v>
+      </c>
+      <c r="S130">
+        <v>1</v>
+      </c>
+      <c r="V130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A131" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C131" s="13">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="D131" s="7">
+        <v>43794</v>
+      </c>
+      <c r="E131" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F131" s="8">
+        <v>43800</v>
+      </c>
+      <c r="G131" s="7">
+        <v>44651</v>
+      </c>
+      <c r="H131" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I130" s="1">
-        <v>44286</v>
-      </c>
-      <c r="J130" s="5">
-        <v>1</v>
-      </c>
-      <c r="K130">
-        <v>1</v>
-      </c>
-      <c r="L130">
-        <v>1</v>
-      </c>
-      <c r="M130">
-        <v>1</v>
-      </c>
-      <c r="V130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+      <c r="I131" s="3">
+        <v>44651</v>
+      </c>
+      <c r="J131" s="9">
+        <v>2</v>
+      </c>
+      <c r="K131" s="2">
+        <v>1</v>
+      </c>
+      <c r="L131" s="2">
+        <v>1</v>
+      </c>
+      <c r="M131" s="2">
+        <v>1</v>
+      </c>
+      <c r="N131" s="2"/>
+      <c r="O131" s="2"/>
+      <c r="P131" s="2"/>
+      <c r="Q131" s="2"/>
+      <c r="R131" s="2"/>
+      <c r="S131" s="2"/>
+      <c r="T131" s="2"/>
+      <c r="U131" s="2"/>
+      <c r="V131" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>19</v>
       </c>
-      <c r="B131" t="s">
-        <v>21</v>
-      </c>
-      <c r="C131">
-        <v>130</v>
-      </c>
-      <c r="D131" s="6">
-        <v>43794</v>
-      </c>
-      <c r="E131" s="1" t="s">
+      <c r="B132" t="s">
+        <v>22</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="0"/>
+        <v>131</v>
+      </c>
+      <c r="D132" s="6">
+        <v>43791</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F131" s="1">
+      <c r="F132" s="1">
         <v>43800</v>
       </c>
-      <c r="G131" s="6">
-        <v>44475</v>
-      </c>
-      <c r="H131" t="s">
-        <v>39</v>
-      </c>
-      <c r="I131" s="1">
-        <v>44469</v>
-      </c>
-      <c r="J131" s="5">
-        <v>1</v>
-      </c>
-      <c r="K131">
-        <v>1</v>
-      </c>
-      <c r="L131">
-        <v>1</v>
-      </c>
-      <c r="M131">
-        <v>1</v>
-      </c>
-      <c r="N131">
-        <v>1</v>
-      </c>
-      <c r="O131">
-        <v>1</v>
-      </c>
-      <c r="P131">
-        <v>1</v>
-      </c>
-      <c r="Q131">
-        <v>1</v>
-      </c>
-      <c r="R131">
-        <v>1</v>
-      </c>
-      <c r="S131">
-        <v>1</v>
-      </c>
-      <c r="V131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C132" s="2">
-        <v>131</v>
-      </c>
-      <c r="D132" s="7">
-        <v>43794</v>
-      </c>
-      <c r="E132" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F132" s="8">
-        <v>43800</v>
-      </c>
-      <c r="G132" s="7">
-        <v>44651</v>
-      </c>
-      <c r="H132" s="2" t="s">
+      <c r="G132" s="6">
+        <v>43915</v>
+      </c>
+      <c r="H132" t="s">
         <v>33</v>
       </c>
-      <c r="I132" s="3">
-        <v>44651</v>
-      </c>
-      <c r="J132" s="9">
-        <v>2</v>
-      </c>
-      <c r="K132" s="2">
-        <v>1</v>
-      </c>
-      <c r="L132" s="2">
-        <v>1</v>
-      </c>
-      <c r="M132" s="2">
-        <v>1</v>
-      </c>
-      <c r="N132" s="2"/>
-      <c r="O132" s="2"/>
-      <c r="P132" s="2"/>
-      <c r="Q132" s="2"/>
-      <c r="R132" s="2"/>
-      <c r="S132" s="2"/>
-      <c r="T132" s="2"/>
-      <c r="U132" s="2"/>
-      <c r="V132" s="2">
+      <c r="I132" s="1">
+        <v>43920</v>
+      </c>
+      <c r="J132" s="5"/>
+      <c r="K132">
+        <v>1</v>
+      </c>
+      <c r="L132">
+        <v>1</v>
+      </c>
+      <c r="M132">
+        <v>1</v>
+      </c>
+      <c r="V132">
         <v>1</v>
       </c>
     </row>
@@ -14880,6 +14891,7 @@
         <v>22</v>
       </c>
       <c r="C133">
+        <f t="shared" si="0"/>
         <v>132</v>
       </c>
       <c r="D133" s="6">
@@ -14892,13 +14904,13 @@
         <v>43800</v>
       </c>
       <c r="G133" s="6">
-        <v>43915</v>
+        <v>44119</v>
       </c>
       <c r="H133" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="I133" s="1">
-        <v>43920</v>
+        <v>44119</v>
       </c>
       <c r="J133" s="5"/>
       <c r="K133">
@@ -14909,6 +14921,27 @@
       </c>
       <c r="M133">
         <v>1</v>
+      </c>
+      <c r="N133">
+        <v>1</v>
+      </c>
+      <c r="O133">
+        <v>1</v>
+      </c>
+      <c r="P133">
+        <v>1</v>
+      </c>
+      <c r="Q133">
+        <v>1</v>
+      </c>
+      <c r="R133">
+        <v>1</v>
+      </c>
+      <c r="S133">
+        <v>1</v>
+      </c>
+      <c r="T133">
+        <v>0.5</v>
       </c>
       <c r="V133">
         <v>1</v>
@@ -14922,6 +14955,7 @@
         <v>22</v>
       </c>
       <c r="C134">
+        <f t="shared" si="0"/>
         <v>133</v>
       </c>
       <c r="D134" s="6">
@@ -14934,15 +14968,17 @@
         <v>43800</v>
       </c>
       <c r="G134" s="6">
-        <v>44119</v>
+        <v>44287</v>
       </c>
       <c r="H134" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I134" s="1">
-        <v>44119</v>
-      </c>
-      <c r="J134" s="5"/>
+        <v>44286</v>
+      </c>
+      <c r="J134" s="5">
+        <v>1</v>
+      </c>
       <c r="K134">
         <v>1</v>
       </c>
@@ -14951,27 +14987,6 @@
       </c>
       <c r="M134">
         <v>1</v>
-      </c>
-      <c r="N134">
-        <v>1</v>
-      </c>
-      <c r="O134">
-        <v>1</v>
-      </c>
-      <c r="P134">
-        <v>1</v>
-      </c>
-      <c r="Q134">
-        <v>1</v>
-      </c>
-      <c r="R134">
-        <v>1</v>
-      </c>
-      <c r="S134">
-        <v>1</v>
-      </c>
-      <c r="T134">
-        <v>0.5</v>
       </c>
       <c r="V134">
         <v>1</v>
@@ -14985,6 +15000,7 @@
         <v>22</v>
       </c>
       <c r="C135">
+        <f t="shared" si="0"/>
         <v>134</v>
       </c>
       <c r="D135" s="6">
@@ -14997,141 +15013,141 @@
         <v>43800</v>
       </c>
       <c r="G135" s="6">
-        <v>44287</v>
+        <v>44477</v>
       </c>
       <c r="H135" t="s">
+        <v>39</v>
+      </c>
+      <c r="I135" s="1">
+        <v>44469</v>
+      </c>
+      <c r="J135" s="5">
+        <v>1</v>
+      </c>
+      <c r="K135">
+        <v>1</v>
+      </c>
+      <c r="L135">
+        <v>1</v>
+      </c>
+      <c r="M135">
+        <v>1</v>
+      </c>
+      <c r="N135">
+        <v>1</v>
+      </c>
+      <c r="O135">
+        <v>1</v>
+      </c>
+      <c r="P135">
+        <v>1</v>
+      </c>
+      <c r="Q135">
+        <v>1</v>
+      </c>
+      <c r="R135">
+        <v>1</v>
+      </c>
+      <c r="S135">
+        <v>1</v>
+      </c>
+      <c r="V135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A136" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C136" s="13">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="D136" s="7">
+        <v>43791</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F136" s="8">
+        <v>43800</v>
+      </c>
+      <c r="G136" s="7">
+        <v>44648</v>
+      </c>
+      <c r="H136" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I135" s="1">
-        <v>44286</v>
-      </c>
-      <c r="J135" s="5">
-        <v>1</v>
-      </c>
-      <c r="K135">
-        <v>1</v>
-      </c>
-      <c r="L135">
-        <v>1</v>
-      </c>
-      <c r="M135">
-        <v>1</v>
-      </c>
-      <c r="V135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
+      <c r="I136" s="3">
+        <v>44651</v>
+      </c>
+      <c r="J136" s="9">
+        <v>2</v>
+      </c>
+      <c r="K136" s="2">
+        <v>1</v>
+      </c>
+      <c r="L136" s="2">
+        <v>1</v>
+      </c>
+      <c r="M136" s="2">
+        <v>1</v>
+      </c>
+      <c r="N136" s="2"/>
+      <c r="O136" s="2"/>
+      <c r="P136" s="2"/>
+      <c r="Q136" s="2"/>
+      <c r="R136" s="2"/>
+      <c r="S136" s="2"/>
+      <c r="T136" s="2"/>
+      <c r="U136" s="2"/>
+      <c r="V136" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>19</v>
       </c>
-      <c r="B136" t="s">
-        <v>22</v>
-      </c>
-      <c r="C136">
-        <v>135</v>
-      </c>
-      <c r="D136" s="6">
-        <v>43791</v>
-      </c>
-      <c r="E136" s="1" t="s">
+      <c r="B137" t="s">
+        <v>23</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="D137" s="6">
+        <v>43790</v>
+      </c>
+      <c r="E137" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F136" s="1">
+      <c r="F137" s="1">
         <v>43800</v>
       </c>
-      <c r="G136" s="6">
-        <v>44477</v>
-      </c>
-      <c r="H136" t="s">
-        <v>39</v>
-      </c>
-      <c r="I136" s="1">
-        <v>44469</v>
-      </c>
-      <c r="J136" s="5">
-        <v>1</v>
-      </c>
-      <c r="K136">
-        <v>1</v>
-      </c>
-      <c r="L136">
-        <v>1</v>
-      </c>
-      <c r="M136">
-        <v>1</v>
-      </c>
-      <c r="N136">
-        <v>1</v>
-      </c>
-      <c r="O136">
-        <v>1</v>
-      </c>
-      <c r="P136">
-        <v>1</v>
-      </c>
-      <c r="Q136">
-        <v>1</v>
-      </c>
-      <c r="R136">
-        <v>1</v>
-      </c>
-      <c r="S136">
-        <v>1</v>
-      </c>
-      <c r="V136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C137" s="2">
-        <v>136</v>
-      </c>
-      <c r="D137" s="7">
-        <v>43791</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F137" s="8">
-        <v>43800</v>
-      </c>
-      <c r="G137" s="7">
-        <v>44648</v>
-      </c>
-      <c r="H137" s="2" t="s">
+      <c r="G137" s="6">
+        <v>43917</v>
+      </c>
+      <c r="H137" t="s">
         <v>33</v>
       </c>
-      <c r="I137" s="3">
-        <v>44651</v>
-      </c>
-      <c r="J137" s="9">
-        <v>2</v>
-      </c>
-      <c r="K137" s="2">
-        <v>1</v>
-      </c>
-      <c r="L137" s="2">
-        <v>1</v>
-      </c>
-      <c r="M137" s="2">
-        <v>1</v>
-      </c>
-      <c r="N137" s="2"/>
-      <c r="O137" s="2"/>
-      <c r="P137" s="2"/>
-      <c r="Q137" s="2"/>
-      <c r="R137" s="2"/>
-      <c r="S137" s="2"/>
-      <c r="T137" s="2"/>
-      <c r="U137" s="2"/>
-      <c r="V137" s="2">
+      <c r="I137" s="1">
+        <v>43920</v>
+      </c>
+      <c r="J137" s="5"/>
+      <c r="K137">
+        <v>1</v>
+      </c>
+      <c r="L137">
+        <v>1</v>
+      </c>
+      <c r="M137">
+        <v>1</v>
+      </c>
+      <c r="V137">
         <v>1</v>
       </c>
     </row>
@@ -15143,6 +15159,7 @@
         <v>23</v>
       </c>
       <c r="C138">
+        <f t="shared" si="0"/>
         <v>137</v>
       </c>
       <c r="D138" s="6">
@@ -15155,13 +15172,13 @@
         <v>43800</v>
       </c>
       <c r="G138" s="6">
-        <v>43917</v>
+        <v>44117</v>
       </c>
       <c r="H138" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="I138" s="1">
-        <v>43920</v>
+        <v>44119</v>
       </c>
       <c r="J138" s="5"/>
       <c r="K138">
@@ -15172,6 +15189,27 @@
       </c>
       <c r="M138">
         <v>1</v>
+      </c>
+      <c r="N138">
+        <v>1</v>
+      </c>
+      <c r="O138">
+        <v>1</v>
+      </c>
+      <c r="P138">
+        <v>1</v>
+      </c>
+      <c r="Q138">
+        <v>1</v>
+      </c>
+      <c r="R138">
+        <v>1</v>
+      </c>
+      <c r="S138">
+        <v>1</v>
+      </c>
+      <c r="T138">
+        <v>0.5</v>
       </c>
       <c r="V138">
         <v>1</v>
@@ -15185,6 +15223,7 @@
         <v>23</v>
       </c>
       <c r="C139">
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
       <c r="D139" s="6">
@@ -15197,155 +15236,133 @@
         <v>43800</v>
       </c>
       <c r="G139" s="6">
-        <v>44117</v>
+        <v>44286</v>
       </c>
       <c r="H139" t="s">
+        <v>33</v>
+      </c>
+      <c r="I139" s="1">
+        <v>44286</v>
+      </c>
+      <c r="J139" s="5">
+        <v>1</v>
+      </c>
+      <c r="K139">
+        <v>1</v>
+      </c>
+      <c r="L139">
+        <v>1</v>
+      </c>
+      <c r="M139">
+        <v>1</v>
+      </c>
+      <c r="V139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C140" s="13">
+        <f t="shared" si="0"/>
+        <v>139</v>
+      </c>
+      <c r="D140" s="7">
+        <v>43790</v>
+      </c>
+      <c r="E140" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F140" s="8">
+        <v>43800</v>
+      </c>
+      <c r="G140" s="7">
+        <v>44482</v>
+      </c>
+      <c r="H140" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="I139" s="1">
-        <v>44119</v>
-      </c>
-      <c r="J139" s="5"/>
-      <c r="K139">
-        <v>1</v>
-      </c>
-      <c r="L139">
-        <v>1</v>
-      </c>
-      <c r="M139">
-        <v>1</v>
-      </c>
-      <c r="N139">
-        <v>1</v>
-      </c>
-      <c r="O139">
-        <v>1</v>
-      </c>
-      <c r="P139">
-        <v>1</v>
-      </c>
-      <c r="Q139">
-        <v>1</v>
-      </c>
-      <c r="R139">
-        <v>1</v>
-      </c>
-      <c r="S139">
-        <v>1</v>
-      </c>
-      <c r="T139">
-        <v>0.5</v>
-      </c>
-      <c r="V139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>19</v>
-      </c>
-      <c r="B140" t="s">
-        <v>23</v>
-      </c>
-      <c r="C140">
-        <v>139</v>
-      </c>
-      <c r="D140" s="6">
-        <v>43790</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F140" s="1">
-        <v>43800</v>
-      </c>
-      <c r="G140" s="6">
-        <v>44286</v>
-      </c>
-      <c r="H140" t="s">
-        <v>33</v>
-      </c>
-      <c r="I140" s="1">
-        <v>44286</v>
-      </c>
-      <c r="J140" s="5">
-        <v>1</v>
-      </c>
-      <c r="K140">
-        <v>1</v>
-      </c>
-      <c r="L140">
-        <v>1</v>
-      </c>
-      <c r="M140">
-        <v>1</v>
-      </c>
-      <c r="V140">
+      <c r="I140" s="3">
+        <v>44484</v>
+      </c>
+      <c r="J140" s="9">
+        <v>1</v>
+      </c>
+      <c r="K140" s="2">
+        <v>1</v>
+      </c>
+      <c r="L140" s="2">
+        <v>1</v>
+      </c>
+      <c r="M140" s="2">
+        <v>1</v>
+      </c>
+      <c r="N140" s="2">
+        <v>1</v>
+      </c>
+      <c r="O140" s="2">
+        <v>1</v>
+      </c>
+      <c r="P140" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q140" s="2">
+        <v>1</v>
+      </c>
+      <c r="R140" s="2">
+        <v>1</v>
+      </c>
+      <c r="S140" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="T140" s="2"/>
+      <c r="U140" s="2"/>
+      <c r="V140" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C141" s="2">
+      <c r="A141" t="s">
+        <v>24</v>
+      </c>
+      <c r="B141" t="s">
+        <v>25</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="D141" s="7">
-        <v>43790</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F141" s="8">
-        <v>43800</v>
-      </c>
-      <c r="G141" s="7">
-        <v>44482</v>
-      </c>
-      <c r="H141" s="2" t="s">
+      <c r="D141" s="6">
+        <v>43686</v>
+      </c>
+      <c r="E141" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F141" s="1">
+        <v>43678</v>
+      </c>
+      <c r="G141" s="6">
+        <v>43781</v>
+      </c>
+      <c r="H141" t="s">
         <v>64</v>
       </c>
-      <c r="I141" s="3">
-        <v>44484</v>
-      </c>
-      <c r="J141" s="9">
-        <v>1</v>
-      </c>
-      <c r="K141" s="2">
-        <v>1</v>
-      </c>
-      <c r="L141" s="2">
-        <v>1</v>
-      </c>
-      <c r="M141" s="2">
-        <v>1</v>
-      </c>
-      <c r="N141" s="2">
-        <v>1</v>
-      </c>
-      <c r="O141" s="2">
-        <v>1</v>
-      </c>
-      <c r="P141" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q141" s="2">
-        <v>1</v>
-      </c>
-      <c r="R141" s="2">
-        <v>1</v>
-      </c>
-      <c r="S141" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="T141" s="2"/>
-      <c r="U141" s="2"/>
-      <c r="V141" s="2">
-        <v>1</v>
+      <c r="I141" s="1">
+        <v>43753</v>
+      </c>
+      <c r="J141" s="5"/>
+      <c r="R141">
+        <v>1</v>
+      </c>
+      <c r="S141">
+        <v>1</v>
+      </c>
+      <c r="T141">
+        <v>0.5</v>
       </c>
     </row>
     <row r="142" spans="1:22" x14ac:dyDescent="0.3">
@@ -15356,6 +15373,7 @@
         <v>25</v>
       </c>
       <c r="C142">
+        <f t="shared" si="0"/>
         <v>141</v>
       </c>
       <c r="D142" s="6">
@@ -15368,15 +15386,24 @@
         <v>43678</v>
       </c>
       <c r="G142" s="6">
-        <v>43781</v>
+        <v>43920</v>
       </c>
       <c r="H142" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I142" s="1">
-        <v>43753</v>
+        <v>43921</v>
       </c>
       <c r="J142" s="5"/>
+      <c r="K142">
+        <v>1</v>
+      </c>
+      <c r="L142">
+        <v>1</v>
+      </c>
+      <c r="M142">
+        <v>1</v>
+      </c>
       <c r="R142">
         <v>1</v>
       </c>
@@ -15384,7 +15411,13 @@
         <v>1</v>
       </c>
       <c r="T142">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="U142">
+        <v>1</v>
+      </c>
+      <c r="V142">
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:22" x14ac:dyDescent="0.3">
@@ -15395,6 +15428,7 @@
         <v>25</v>
       </c>
       <c r="C143">
+        <f t="shared" si="0"/>
         <v>142</v>
       </c>
       <c r="D143" s="6">
@@ -15407,37 +15441,21 @@
         <v>43678</v>
       </c>
       <c r="G143" s="6">
-        <v>43920</v>
+        <v>44105</v>
       </c>
       <c r="H143" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I143" s="1">
-        <v>43921</v>
-      </c>
-      <c r="J143" s="5"/>
-      <c r="K143">
-        <v>1</v>
-      </c>
-      <c r="L143">
-        <v>1</v>
-      </c>
-      <c r="M143">
+        <v>44104</v>
+      </c>
+      <c r="J143" s="5">
         <v>1</v>
       </c>
       <c r="R143">
         <v>1</v>
       </c>
       <c r="S143">
-        <v>1</v>
-      </c>
-      <c r="T143">
-        <v>1</v>
-      </c>
-      <c r="U143">
-        <v>1</v>
-      </c>
-      <c r="V143">
         <v>1</v>
       </c>
     </row>
@@ -15449,6 +15467,7 @@
         <v>25</v>
       </c>
       <c r="C144">
+        <f t="shared" si="0"/>
         <v>143</v>
       </c>
       <c r="D144" s="6">
@@ -15461,7 +15480,7 @@
         <v>43678</v>
       </c>
       <c r="G144" s="6">
-        <v>44105</v>
+        <v>44108</v>
       </c>
       <c r="H144" t="s">
         <v>39</v>
@@ -15487,6 +15506,7 @@
         <v>25</v>
       </c>
       <c r="C145">
+        <f t="shared" si="0"/>
         <v>144</v>
       </c>
       <c r="D145" s="6">
@@ -15499,21 +15519,39 @@
         <v>43678</v>
       </c>
       <c r="G145" s="6">
-        <v>44108</v>
+        <v>44267</v>
       </c>
       <c r="H145" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="I145" s="1">
-        <v>44104</v>
+        <v>44270</v>
       </c>
       <c r="J145" s="5">
         <v>1</v>
       </c>
+      <c r="K145">
+        <v>1</v>
+      </c>
+      <c r="L145">
+        <v>1</v>
+      </c>
+      <c r="M145">
+        <v>0.5</v>
+      </c>
       <c r="R145">
         <v>1</v>
       </c>
       <c r="S145">
+        <v>1</v>
+      </c>
+      <c r="T145">
+        <v>1</v>
+      </c>
+      <c r="U145">
+        <v>1</v>
+      </c>
+      <c r="V145">
         <v>1</v>
       </c>
     </row>
@@ -15525,6 +15563,7 @@
         <v>25</v>
       </c>
       <c r="C146">
+        <f t="shared" si="0"/>
         <v>145</v>
       </c>
       <c r="D146" s="6">
@@ -15537,25 +15576,16 @@
         <v>43678</v>
       </c>
       <c r="G146" s="6">
-        <v>44267</v>
+        <v>44482</v>
       </c>
       <c r="H146" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="I146" s="1">
-        <v>44270</v>
+        <v>44484</v>
       </c>
       <c r="J146" s="5">
-        <v>1</v>
-      </c>
-      <c r="K146">
-        <v>1</v>
-      </c>
-      <c r="L146">
-        <v>1</v>
-      </c>
-      <c r="M146">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="R146">
         <v>1</v>
@@ -15564,13 +15594,7 @@
         <v>1</v>
       </c>
       <c r="T146">
-        <v>1</v>
-      </c>
-      <c r="U146">
-        <v>1</v>
-      </c>
-      <c r="V146">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="147" spans="1:22" x14ac:dyDescent="0.3">
@@ -15581,6 +15605,7 @@
         <v>25</v>
       </c>
       <c r="C147">
+        <f t="shared" si="0"/>
         <v>146</v>
       </c>
       <c r="D147" s="6">
@@ -15593,7 +15618,7 @@
         <v>43678</v>
       </c>
       <c r="G147" s="6">
-        <v>44482</v>
+        <v>44483</v>
       </c>
       <c r="H147" t="s">
         <v>64</v>
@@ -15622,6 +15647,7 @@
         <v>25</v>
       </c>
       <c r="C148">
+        <f t="shared" si="0"/>
         <v>147</v>
       </c>
       <c r="D148" s="6">
@@ -15634,17 +15660,26 @@
         <v>43678</v>
       </c>
       <c r="G148" s="6">
-        <v>44483</v>
+        <v>44650</v>
       </c>
       <c r="H148" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="I148" s="1">
-        <v>44484</v>
+        <v>44651</v>
       </c>
       <c r="J148" s="5">
         <v>2</v>
       </c>
+      <c r="K148">
+        <v>1</v>
+      </c>
+      <c r="L148">
+        <v>1</v>
+      </c>
+      <c r="M148">
+        <v>1</v>
+      </c>
       <c r="R148">
         <v>1</v>
       </c>
@@ -15652,122 +15687,113 @@
         <v>1</v>
       </c>
       <c r="T148">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="U148">
+        <v>1</v>
+      </c>
+      <c r="V148">
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+      <c r="A149" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C149">
+      <c r="C149" s="13">
+        <f t="shared" si="0"/>
         <v>148</v>
       </c>
-      <c r="D149" s="6">
+      <c r="D149" s="7">
         <v>43686</v>
       </c>
-      <c r="E149" s="1" t="s">
+      <c r="E149" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F149" s="1">
+      <c r="F149" s="8">
         <v>43678</v>
       </c>
-      <c r="G149" s="6">
-        <v>44650</v>
-      </c>
-      <c r="H149" t="s">
+      <c r="G149" s="7">
+        <v>44651</v>
+      </c>
+      <c r="H149" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I149" s="1">
+      <c r="I149" s="3">
         <v>44651</v>
       </c>
-      <c r="J149" s="5">
+      <c r="J149" s="9">
         <v>2</v>
       </c>
-      <c r="K149">
-        <v>1</v>
-      </c>
-      <c r="L149">
-        <v>1</v>
-      </c>
-      <c r="M149">
-        <v>1</v>
-      </c>
-      <c r="R149">
-        <v>1</v>
-      </c>
-      <c r="S149">
-        <v>1</v>
-      </c>
-      <c r="T149">
-        <v>1</v>
-      </c>
-      <c r="U149">
-        <v>1</v>
-      </c>
-      <c r="V149">
+      <c r="K149" s="2">
+        <v>1</v>
+      </c>
+      <c r="L149" s="2">
+        <v>1</v>
+      </c>
+      <c r="M149" s="2">
+        <v>1</v>
+      </c>
+      <c r="N149" s="2"/>
+      <c r="O149" s="2"/>
+      <c r="P149" s="2"/>
+      <c r="Q149" s="2"/>
+      <c r="R149" s="2">
+        <v>1</v>
+      </c>
+      <c r="S149" s="2">
+        <v>1</v>
+      </c>
+      <c r="T149" s="2">
+        <v>1</v>
+      </c>
+      <c r="U149" s="2">
+        <v>1</v>
+      </c>
+      <c r="V149" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
+      <c r="A150" t="s">
         <v>24</v>
       </c>
-      <c r="B150" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C150" s="2">
+      <c r="B150" t="s">
+        <v>26</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="0"/>
         <v>149</v>
       </c>
-      <c r="D150" s="7">
+      <c r="D150" s="6">
         <v>43686</v>
       </c>
-      <c r="E150" s="3" t="s">
+      <c r="E150" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F150" s="8">
+      <c r="F150" s="1">
         <v>43678</v>
       </c>
-      <c r="G150" s="7">
-        <v>44651</v>
-      </c>
-      <c r="H150" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I150" s="3">
-        <v>44651</v>
-      </c>
-      <c r="J150" s="9">
-        <v>2</v>
-      </c>
-      <c r="K150" s="2">
-        <v>1</v>
-      </c>
-      <c r="L150" s="2">
-        <v>1</v>
-      </c>
-      <c r="M150" s="2">
-        <v>1</v>
-      </c>
-      <c r="N150" s="2"/>
-      <c r="O150" s="2"/>
-      <c r="P150" s="2"/>
-      <c r="Q150" s="2"/>
-      <c r="R150" s="2">
-        <v>1</v>
-      </c>
-      <c r="S150" s="2">
-        <v>1</v>
-      </c>
-      <c r="T150" s="2">
-        <v>1</v>
-      </c>
-      <c r="U150" s="2">
-        <v>1</v>
-      </c>
-      <c r="V150" s="2">
+      <c r="G150" s="6">
+        <v>43776</v>
+      </c>
+      <c r="H150" t="s">
+        <v>40</v>
+      </c>
+      <c r="I150" s="1">
+        <v>43769</v>
+      </c>
+      <c r="J150" s="5"/>
+      <c r="R150">
+        <v>1</v>
+      </c>
+      <c r="S150">
+        <v>1</v>
+      </c>
+      <c r="T150">
         <v>1</v>
       </c>
     </row>
@@ -15779,6 +15805,7 @@
         <v>26</v>
       </c>
       <c r="C151">
+        <f t="shared" si="0"/>
         <v>150</v>
       </c>
       <c r="D151" s="6">
@@ -15791,15 +15818,24 @@
         <v>43678</v>
       </c>
       <c r="G151" s="6">
-        <v>43776</v>
+        <v>43923</v>
       </c>
       <c r="H151" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I151" s="1">
-        <v>43769</v>
+        <v>43921</v>
       </c>
       <c r="J151" s="5"/>
+      <c r="K151">
+        <v>1</v>
+      </c>
+      <c r="L151">
+        <v>1</v>
+      </c>
+      <c r="M151">
+        <v>1</v>
+      </c>
       <c r="R151">
         <v>1</v>
       </c>
@@ -15807,6 +15843,12 @@
         <v>1</v>
       </c>
       <c r="T151">
+        <v>1</v>
+      </c>
+      <c r="U151">
+        <v>1</v>
+      </c>
+      <c r="V151">
         <v>1</v>
       </c>
     </row>
@@ -15818,6 +15860,7 @@
         <v>26</v>
       </c>
       <c r="C152">
+        <f t="shared" si="0"/>
         <v>151</v>
       </c>
       <c r="D152" s="6">
@@ -15830,37 +15873,21 @@
         <v>43678</v>
       </c>
       <c r="G152" s="6">
-        <v>43923</v>
+        <v>44104</v>
       </c>
       <c r="H152" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I152" s="1">
-        <v>43921</v>
-      </c>
-      <c r="J152" s="5"/>
-      <c r="K152">
-        <v>1</v>
-      </c>
-      <c r="L152">
-        <v>1</v>
-      </c>
-      <c r="M152">
+        <v>44104</v>
+      </c>
+      <c r="J152" s="5">
         <v>1</v>
       </c>
       <c r="R152">
         <v>1</v>
       </c>
       <c r="S152">
-        <v>1</v>
-      </c>
-      <c r="T152">
-        <v>1</v>
-      </c>
-      <c r="U152">
-        <v>1</v>
-      </c>
-      <c r="V152">
         <v>1</v>
       </c>
     </row>
@@ -15872,6 +15899,7 @@
         <v>26</v>
       </c>
       <c r="C153">
+        <f t="shared" si="0"/>
         <v>152</v>
       </c>
       <c r="D153" s="6">
@@ -15884,21 +15912,39 @@
         <v>43678</v>
       </c>
       <c r="G153" s="6">
-        <v>44104</v>
+        <v>44265</v>
       </c>
       <c r="H153" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="I153" s="1">
-        <v>44104</v>
+        <v>44270</v>
       </c>
       <c r="J153" s="5">
         <v>1</v>
       </c>
+      <c r="K153">
+        <v>1</v>
+      </c>
+      <c r="L153">
+        <v>1</v>
+      </c>
+      <c r="M153">
+        <v>0.5</v>
+      </c>
       <c r="R153">
         <v>1</v>
       </c>
       <c r="S153">
+        <v>1</v>
+      </c>
+      <c r="T153">
+        <v>1</v>
+      </c>
+      <c r="U153">
+        <v>1</v>
+      </c>
+      <c r="V153">
         <v>1</v>
       </c>
     </row>
@@ -15910,6 +15956,7 @@
         <v>26</v>
       </c>
       <c r="C154">
+        <f t="shared" si="0"/>
         <v>153</v>
       </c>
       <c r="D154" s="6">
@@ -15922,7 +15969,7 @@
         <v>43678</v>
       </c>
       <c r="G154" s="6">
-        <v>44265</v>
+        <v>44266</v>
       </c>
       <c r="H154" t="s">
         <v>61</v>
@@ -15966,6 +16013,7 @@
         <v>26</v>
       </c>
       <c r="C155">
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="D155" s="6">
@@ -15978,39 +16026,21 @@
         <v>43678</v>
       </c>
       <c r="G155" s="6">
-        <v>44266</v>
+        <v>44475</v>
       </c>
       <c r="H155" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="I155" s="1">
-        <v>44270</v>
+        <v>44469</v>
       </c>
       <c r="J155" s="5">
-        <v>1</v>
-      </c>
-      <c r="K155">
-        <v>1</v>
-      </c>
-      <c r="L155">
-        <v>1</v>
-      </c>
-      <c r="M155">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="R155">
         <v>1</v>
       </c>
       <c r="S155">
-        <v>1</v>
-      </c>
-      <c r="T155">
-        <v>1</v>
-      </c>
-      <c r="U155">
-        <v>1</v>
-      </c>
-      <c r="V155">
         <v>1</v>
       </c>
     </row>
@@ -16022,6 +16052,7 @@
         <v>26</v>
       </c>
       <c r="C156">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
       <c r="D156" s="6">
@@ -16034,7 +16065,7 @@
         <v>43678</v>
       </c>
       <c r="G156" s="6">
-        <v>44475</v>
+        <v>44476</v>
       </c>
       <c r="H156" t="s">
         <v>39</v>
@@ -16060,6 +16091,7 @@
         <v>26</v>
       </c>
       <c r="C157">
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="D157" s="6">
@@ -16072,7 +16104,7 @@
         <v>43678</v>
       </c>
       <c r="G157" s="6">
-        <v>44476</v>
+        <v>44477</v>
       </c>
       <c r="H157" t="s">
         <v>39</v>
@@ -16098,6 +16130,7 @@
         <v>26</v>
       </c>
       <c r="C158">
+        <f t="shared" si="0"/>
         <v>157</v>
       </c>
       <c r="D158" s="6">
@@ -16110,7 +16143,7 @@
         <v>43678</v>
       </c>
       <c r="G158" s="6">
-        <v>44477</v>
+        <v>44478</v>
       </c>
       <c r="H158" t="s">
         <v>39</v>
@@ -16136,6 +16169,7 @@
         <v>26</v>
       </c>
       <c r="C159">
+        <f t="shared" si="0"/>
         <v>158</v>
       </c>
       <c r="D159" s="6">
@@ -16148,21 +16182,39 @@
         <v>43678</v>
       </c>
       <c r="G159" s="6">
-        <v>44478</v>
+        <v>44643</v>
       </c>
       <c r="H159" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I159" s="1">
-        <v>44469</v>
+        <v>44651</v>
       </c>
       <c r="J159" s="5">
         <v>2</v>
       </c>
+      <c r="K159">
+        <v>1</v>
+      </c>
+      <c r="L159">
+        <v>1</v>
+      </c>
+      <c r="M159">
+        <v>1</v>
+      </c>
       <c r="R159">
         <v>1</v>
       </c>
       <c r="S159">
+        <v>1</v>
+      </c>
+      <c r="T159">
+        <v>1</v>
+      </c>
+      <c r="U159">
+        <v>1</v>
+      </c>
+      <c r="V159">
         <v>1</v>
       </c>
     </row>
@@ -16174,6 +16226,7 @@
         <v>26</v>
       </c>
       <c r="C160">
+        <f t="shared" si="0"/>
         <v>159</v>
       </c>
       <c r="D160" s="6">
@@ -16182,11 +16235,11 @@
       <c r="E160" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F160" s="1">
+      <c r="F160" s="10">
         <v>43678</v>
       </c>
       <c r="G160" s="6">
-        <v>44643</v>
+        <v>44644</v>
       </c>
       <c r="H160" t="s">
         <v>33</v>
@@ -16223,119 +16276,98 @@
       </c>
     </row>
     <row r="161" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A161" t="s">
+      <c r="A161" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C161">
+      <c r="C161" s="13">
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="D161" s="6">
+      <c r="D161" s="7">
         <v>43686</v>
       </c>
-      <c r="E161" s="1" t="s">
+      <c r="E161" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F161" s="10">
+      <c r="F161" s="8">
         <v>43678</v>
       </c>
-      <c r="G161" s="6">
-        <v>44644</v>
-      </c>
-      <c r="H161" t="s">
+      <c r="G161" s="7">
+        <v>44648</v>
+      </c>
+      <c r="H161" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I161" s="1">
+      <c r="I161" s="3">
         <v>44651</v>
       </c>
-      <c r="J161" s="5">
+      <c r="J161" s="9">
         <v>2</v>
       </c>
-      <c r="K161">
-        <v>1</v>
-      </c>
-      <c r="L161">
-        <v>1</v>
-      </c>
-      <c r="M161">
-        <v>1</v>
-      </c>
-      <c r="R161">
-        <v>1</v>
-      </c>
-      <c r="S161">
-        <v>1</v>
-      </c>
-      <c r="T161">
-        <v>1</v>
-      </c>
-      <c r="U161">
-        <v>1</v>
-      </c>
-      <c r="V161">
+      <c r="K161" s="2">
+        <v>1</v>
+      </c>
+      <c r="L161" s="2">
+        <v>1</v>
+      </c>
+      <c r="M161" s="2">
+        <v>1</v>
+      </c>
+      <c r="N161" s="2"/>
+      <c r="O161" s="2"/>
+      <c r="P161" s="2"/>
+      <c r="Q161" s="2"/>
+      <c r="R161" s="2">
+        <v>1</v>
+      </c>
+      <c r="S161" s="2">
+        <v>1</v>
+      </c>
+      <c r="T161" s="2">
+        <v>1</v>
+      </c>
+      <c r="U161" s="2">
+        <v>1</v>
+      </c>
+      <c r="V161" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="162" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C162" s="2">
+      <c r="A162" t="s">
+        <v>27</v>
+      </c>
+      <c r="B162" t="s">
+        <v>28</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="0"/>
         <v>161</v>
       </c>
-      <c r="D162" s="7">
-        <v>43686</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F162" s="8">
-        <v>43678</v>
-      </c>
-      <c r="G162" s="7">
-        <v>44648</v>
-      </c>
-      <c r="H162" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="I162" s="3">
-        <v>44651</v>
-      </c>
-      <c r="J162" s="9">
-        <v>2</v>
-      </c>
-      <c r="K162" s="2">
-        <v>1</v>
-      </c>
-      <c r="L162" s="2">
-        <v>1</v>
-      </c>
-      <c r="M162" s="2">
-        <v>1</v>
-      </c>
-      <c r="N162" s="2"/>
-      <c r="O162" s="2"/>
-      <c r="P162" s="2"/>
-      <c r="Q162" s="2"/>
-      <c r="R162" s="2">
-        <v>1</v>
-      </c>
-      <c r="S162" s="2">
-        <v>1</v>
-      </c>
-      <c r="T162" s="2">
-        <v>1</v>
-      </c>
-      <c r="U162" s="2">
-        <v>1</v>
-      </c>
-      <c r="V162" s="2">
-        <v>1</v>
+      <c r="D162" s="6">
+        <v>43390</v>
+      </c>
+      <c r="E162" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F162" s="1">
+        <v>43388</v>
+      </c>
+      <c r="G162" s="6">
+        <v>43406</v>
+      </c>
+      <c r="H162" t="s">
+        <v>40</v>
+      </c>
+      <c r="I162" s="1">
+        <v>43404</v>
+      </c>
+      <c r="J162" s="5"/>
+      <c r="T162">
+        <v>0.5</v>
       </c>
     </row>
     <row r="163" spans="1:22" x14ac:dyDescent="0.3">
@@ -16346,6 +16378,7 @@
         <v>28</v>
       </c>
       <c r="C163">
+        <f t="shared" si="0"/>
         <v>162</v>
       </c>
       <c r="D163" s="6">
@@ -16358,16 +16391,19 @@
         <v>43388</v>
       </c>
       <c r="G163" s="6">
-        <v>43406</v>
+        <v>43420</v>
       </c>
       <c r="H163" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="I163" s="1">
-        <v>43404</v>
+        <v>43419</v>
       </c>
       <c r="J163" s="5"/>
       <c r="T163">
+        <v>0.5</v>
+      </c>
+      <c r="U163">
         <v>0.5</v>
       </c>
     </row>
@@ -16379,6 +16415,7 @@
         <v>28</v>
       </c>
       <c r="C164">
+        <f t="shared" si="0"/>
         <v>163</v>
       </c>
       <c r="D164" s="6">
@@ -16391,19 +16428,25 @@
         <v>43388</v>
       </c>
       <c r="G164" s="6">
-        <v>43420</v>
+        <v>43445</v>
       </c>
       <c r="H164" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I164" s="1">
-        <v>43419</v>
+        <v>43449</v>
       </c>
       <c r="J164" s="5"/>
+      <c r="M164" t="s">
+        <v>73</v>
+      </c>
       <c r="T164">
         <v>0.5</v>
       </c>
       <c r="U164">
+        <v>1</v>
+      </c>
+      <c r="V164">
         <v>0.5</v>
       </c>
     </row>
@@ -16415,6 +16458,7 @@
         <v>28</v>
       </c>
       <c r="C165">
+        <f t="shared" si="0"/>
         <v>164</v>
       </c>
       <c r="D165" s="6">
@@ -16427,17 +16471,23 @@
         <v>43388</v>
       </c>
       <c r="G165" s="6">
-        <v>43445</v>
+        <v>43546</v>
       </c>
       <c r="H165" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="I165" s="1">
-        <v>43449</v>
+        <v>43555</v>
       </c>
       <c r="J165" s="5"/>
-      <c r="M165" t="s">
-        <v>73</v>
+      <c r="K165">
+        <v>1</v>
+      </c>
+      <c r="L165">
+        <v>1</v>
+      </c>
+      <c r="M165">
+        <v>1</v>
       </c>
       <c r="T165">
         <v>0.5</v>
@@ -16446,7 +16496,7 @@
         <v>1</v>
       </c>
       <c r="V165">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:22" x14ac:dyDescent="0.3">
@@ -16457,6 +16507,7 @@
         <v>28</v>
       </c>
       <c r="C166">
+        <f t="shared" si="0"/>
         <v>165</v>
       </c>
       <c r="D166" s="6">
@@ -16469,7 +16520,7 @@
         <v>43388</v>
       </c>
       <c r="G166" s="6">
-        <v>43546</v>
+        <v>43560</v>
       </c>
       <c r="H166" t="s">
         <v>33</v>
@@ -16505,6 +16556,7 @@
         <v>28</v>
       </c>
       <c r="C167">
+        <f t="shared" si="0"/>
         <v>166</v>
       </c>
       <c r="D167" s="6">
@@ -16517,13 +16569,13 @@
         <v>43388</v>
       </c>
       <c r="G167" s="6">
-        <v>43560</v>
+        <v>43580</v>
       </c>
       <c r="H167" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I167" s="1">
-        <v>43555</v>
+        <v>43585</v>
       </c>
       <c r="J167" s="5"/>
       <c r="K167">
@@ -16533,6 +16585,9 @@
         <v>1</v>
       </c>
       <c r="M167">
+        <v>1</v>
+      </c>
+      <c r="N167">
         <v>1</v>
       </c>
       <c r="T167">
@@ -16553,6 +16608,7 @@
         <v>28</v>
       </c>
       <c r="C168">
+        <f t="shared" si="0"/>
         <v>167</v>
       </c>
       <c r="D168" s="6">
@@ -16565,13 +16621,13 @@
         <v>43388</v>
       </c>
       <c r="G168" s="6">
-        <v>43580</v>
+        <v>43602</v>
       </c>
       <c r="H168" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="I168" s="1">
-        <v>43585</v>
+        <v>43600</v>
       </c>
       <c r="J168" s="5"/>
       <c r="K168">
@@ -16585,6 +16641,9 @@
       </c>
       <c r="N168">
         <v>1</v>
+      </c>
+      <c r="O168">
+        <v>0.5</v>
       </c>
       <c r="T168">
         <v>0.5</v>
@@ -16604,6 +16663,7 @@
         <v>28</v>
       </c>
       <c r="C169">
+        <f t="shared" si="0"/>
         <v>168</v>
       </c>
       <c r="D169" s="6">
@@ -16616,13 +16676,13 @@
         <v>43388</v>
       </c>
       <c r="G169" s="6">
-        <v>43602</v>
+        <v>43629</v>
       </c>
       <c r="H169" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I169" s="1">
-        <v>43600</v>
+        <v>43631</v>
       </c>
       <c r="J169" s="5"/>
       <c r="K169">
@@ -16638,6 +16698,9 @@
         <v>1</v>
       </c>
       <c r="O169">
+        <v>1</v>
+      </c>
+      <c r="P169">
         <v>0.5</v>
       </c>
       <c r="T169">
@@ -16658,6 +16721,7 @@
         <v>28</v>
       </c>
       <c r="C170">
+        <f t="shared" si="0"/>
         <v>169</v>
       </c>
       <c r="D170" s="6">
@@ -16670,13 +16734,13 @@
         <v>43388</v>
       </c>
       <c r="G170" s="6">
-        <v>43629</v>
+        <v>43670</v>
       </c>
       <c r="H170" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="I170" s="1">
-        <v>43631</v>
+        <v>43677</v>
       </c>
       <c r="J170" s="5"/>
       <c r="K170">
@@ -16695,7 +16759,10 @@
         <v>1</v>
       </c>
       <c r="P170">
-        <v>0.5</v>
+        <v>1</v>
+      </c>
+      <c r="Q170">
+        <v>1</v>
       </c>
       <c r="T170">
         <v>0.5</v>
@@ -16708,124 +16775,99 @@
       </c>
     </row>
     <row r="171" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A171" t="s">
+      <c r="A171" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C171">
+      <c r="C171" s="13">
+        <f t="shared" si="0"/>
         <v>170</v>
       </c>
-      <c r="D171" s="6">
+      <c r="D171" s="7">
         <v>43390</v>
       </c>
-      <c r="E171" s="1" t="s">
+      <c r="E171" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F171" s="1">
+      <c r="F171" s="8">
         <v>43388</v>
       </c>
-      <c r="G171" s="6">
-        <v>43670</v>
-      </c>
-      <c r="H171" t="s">
-        <v>37</v>
-      </c>
-      <c r="I171" s="1">
-        <v>43677</v>
-      </c>
-      <c r="J171" s="5"/>
-      <c r="K171">
-        <v>1</v>
-      </c>
-      <c r="L171">
-        <v>1</v>
-      </c>
-      <c r="M171">
-        <v>1</v>
-      </c>
-      <c r="N171">
-        <v>1</v>
-      </c>
-      <c r="O171">
-        <v>1</v>
-      </c>
-      <c r="P171">
-        <v>1</v>
-      </c>
-      <c r="Q171">
-        <v>1</v>
-      </c>
-      <c r="T171">
-        <v>0.5</v>
-      </c>
-      <c r="U171">
-        <v>1</v>
-      </c>
-      <c r="V171">
+      <c r="G171" s="7">
+        <v>44375</v>
+      </c>
+      <c r="H171" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I171" s="3">
+        <v>44377</v>
+      </c>
+      <c r="J171" s="9">
+        <v>2</v>
+      </c>
+      <c r="K171" s="2">
+        <v>1</v>
+      </c>
+      <c r="L171" s="2">
+        <v>1</v>
+      </c>
+      <c r="M171" s="2">
+        <v>1</v>
+      </c>
+      <c r="N171" s="2">
+        <v>1</v>
+      </c>
+      <c r="O171" s="2">
+        <v>1</v>
+      </c>
+      <c r="P171" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q171" s="2"/>
+      <c r="R171" s="2"/>
+      <c r="S171" s="2"/>
+      <c r="T171" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="U171" s="2">
+        <v>1</v>
+      </c>
+      <c r="V171" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="172" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A172" s="2" t="s">
+      <c r="A172" t="s">
         <v>27</v>
       </c>
-      <c r="B172" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C172" s="2">
+      <c r="B172" t="s">
+        <v>29</v>
+      </c>
+      <c r="C172">
+        <f t="shared" si="0"/>
         <v>171</v>
       </c>
-      <c r="D172" s="7">
-        <v>43390</v>
-      </c>
-      <c r="E172" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F172" s="8">
-        <v>43388</v>
-      </c>
-      <c r="G172" s="7">
-        <v>44375</v>
-      </c>
-      <c r="H172" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I172" s="3">
-        <v>44377</v>
-      </c>
-      <c r="J172" s="9">
-        <v>2</v>
-      </c>
-      <c r="K172" s="2">
-        <v>1</v>
-      </c>
-      <c r="L172" s="2">
-        <v>1</v>
-      </c>
-      <c r="M172" s="2">
-        <v>1</v>
-      </c>
-      <c r="N172" s="2">
-        <v>1</v>
-      </c>
-      <c r="O172" s="2">
-        <v>1</v>
-      </c>
-      <c r="P172" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q172" s="2"/>
-      <c r="R172" s="2"/>
-      <c r="S172" s="2"/>
-      <c r="T172" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="U172" s="2">
-        <v>1</v>
-      </c>
-      <c r="V172" s="2">
+      <c r="D172" s="6">
+        <v>43404</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F172" s="1">
+        <v>43405</v>
+      </c>
+      <c r="G172" s="6">
+        <v>43431</v>
+      </c>
+      <c r="H172" t="s">
+        <v>41</v>
+      </c>
+      <c r="I172" s="1">
+        <v>43434</v>
+      </c>
+      <c r="J172" s="5"/>
+      <c r="U172">
         <v>1</v>
       </c>
     </row>
@@ -16837,6 +16879,7 @@
         <v>29</v>
       </c>
       <c r="C173">
+        <f t="shared" si="0"/>
         <v>172</v>
       </c>
       <c r="D173" s="6">
@@ -16849,17 +16892,20 @@
         <v>43405</v>
       </c>
       <c r="G173" s="6">
-        <v>43431</v>
+        <v>43446</v>
       </c>
       <c r="H173" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="I173" s="1">
-        <v>43434</v>
+        <v>43449</v>
       </c>
       <c r="J173" s="5"/>
       <c r="U173">
         <v>1</v>
+      </c>
+      <c r="V173">
+        <v>0.5</v>
       </c>
     </row>
     <row r="174" spans="1:22" x14ac:dyDescent="0.3">
@@ -16870,6 +16916,7 @@
         <v>29</v>
       </c>
       <c r="C174">
+        <f t="shared" si="0"/>
         <v>173</v>
       </c>
       <c r="D174" s="6">
@@ -16882,20 +16929,29 @@
         <v>43405</v>
       </c>
       <c r="G174" s="6">
-        <v>43446</v>
+        <v>43553</v>
       </c>
       <c r="H174" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="I174" s="1">
-        <v>43449</v>
+        <v>43555</v>
       </c>
       <c r="J174" s="5"/>
+      <c r="K174">
+        <v>1</v>
+      </c>
+      <c r="L174">
+        <v>1</v>
+      </c>
+      <c r="M174">
+        <v>1</v>
+      </c>
       <c r="U174">
         <v>1</v>
       </c>
       <c r="V174">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175" spans="1:22" x14ac:dyDescent="0.3">
@@ -16906,6 +16962,7 @@
         <v>29</v>
       </c>
       <c r="C175">
+        <f t="shared" si="0"/>
         <v>174</v>
       </c>
       <c r="D175" s="6">
@@ -16918,13 +16975,13 @@
         <v>43405</v>
       </c>
       <c r="G175" s="6">
-        <v>43553</v>
+        <v>43574</v>
       </c>
       <c r="H175" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="I175" s="1">
-        <v>43555</v>
+        <v>43570</v>
       </c>
       <c r="J175" s="5"/>
       <c r="K175">
@@ -16935,6 +16992,9 @@
       </c>
       <c r="M175">
         <v>1</v>
+      </c>
+      <c r="N175">
+        <v>0.5</v>
       </c>
       <c r="U175">
         <v>1</v>
@@ -16951,6 +17011,7 @@
         <v>29</v>
       </c>
       <c r="C176">
+        <f t="shared" si="0"/>
         <v>175</v>
       </c>
       <c r="D176" s="6">
@@ -16963,13 +17024,13 @@
         <v>43405</v>
       </c>
       <c r="G176" s="6">
-        <v>43574</v>
+        <v>43594</v>
       </c>
       <c r="H176" t="s">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="I176" s="1">
-        <v>43570</v>
+        <v>43585</v>
       </c>
       <c r="J176" s="5"/>
       <c r="K176">
@@ -16982,7 +17043,7 @@
         <v>1</v>
       </c>
       <c r="N176">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U176">
         <v>1</v>
@@ -16999,6 +17060,7 @@
         <v>29</v>
       </c>
       <c r="C177">
+        <f t="shared" si="0"/>
         <v>176</v>
       </c>
       <c r="D177" s="6">
@@ -17011,13 +17073,13 @@
         <v>43405</v>
       </c>
       <c r="G177" s="6">
-        <v>43594</v>
+        <v>43613</v>
       </c>
       <c r="H177" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I177" s="1">
-        <v>43585</v>
+        <v>43616</v>
       </c>
       <c r="J177" s="5"/>
       <c r="K177">
@@ -17030,6 +17092,9 @@
         <v>1</v>
       </c>
       <c r="N177">
+        <v>1</v>
+      </c>
+      <c r="O177">
         <v>1</v>
       </c>
       <c r="U177">
@@ -17047,6 +17112,7 @@
         <v>29</v>
       </c>
       <c r="C178">
+        <f t="shared" si="0"/>
         <v>177</v>
       </c>
       <c r="D178" s="6">
@@ -17059,13 +17125,13 @@
         <v>43405</v>
       </c>
       <c r="G178" s="6">
-        <v>43613</v>
+        <v>43647</v>
       </c>
       <c r="H178" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I178" s="1">
-        <v>43616</v>
+        <v>43646</v>
       </c>
       <c r="J178" s="5"/>
       <c r="K178">
@@ -17081,6 +17147,9 @@
         <v>1</v>
       </c>
       <c r="O178">
+        <v>1</v>
+      </c>
+      <c r="P178">
         <v>1</v>
       </c>
       <c r="U178">
@@ -17098,6 +17167,7 @@
         <v>29</v>
       </c>
       <c r="C179">
+        <f t="shared" si="0"/>
         <v>178</v>
       </c>
       <c r="D179" s="6">
@@ -17110,13 +17180,13 @@
         <v>43405</v>
       </c>
       <c r="G179" s="6">
-        <v>43647</v>
+        <v>43684</v>
       </c>
       <c r="H179" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I179" s="1">
-        <v>43646</v>
+        <v>43677</v>
       </c>
       <c r="J179" s="5"/>
       <c r="K179">
@@ -17137,6 +17207,9 @@
       <c r="P179">
         <v>1</v>
       </c>
+      <c r="Q179">
+        <v>1</v>
+      </c>
       <c r="U179">
         <v>1</v>
       </c>
@@ -17145,120 +17218,98 @@
       </c>
     </row>
     <row r="180" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A180" t="s">
+      <c r="A180" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C180">
+      <c r="C180" s="13">
+        <f t="shared" si="0"/>
         <v>179</v>
       </c>
-      <c r="D180" s="6">
+      <c r="D180" s="7">
         <v>43404</v>
       </c>
-      <c r="E180" s="1" t="s">
+      <c r="E180" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F180" s="1">
+      <c r="F180" s="8">
         <v>43405</v>
       </c>
-      <c r="G180" s="6">
-        <v>43684</v>
-      </c>
-      <c r="H180" t="s">
-        <v>37</v>
-      </c>
-      <c r="I180" s="1">
-        <v>43677</v>
-      </c>
-      <c r="J180" s="5"/>
-      <c r="K180">
-        <v>1</v>
-      </c>
-      <c r="L180">
-        <v>1</v>
-      </c>
-      <c r="M180">
-        <v>1</v>
-      </c>
-      <c r="N180">
-        <v>1</v>
-      </c>
-      <c r="O180">
-        <v>1</v>
-      </c>
-      <c r="P180">
-        <v>1</v>
-      </c>
-      <c r="Q180">
-        <v>1</v>
-      </c>
-      <c r="U180">
-        <v>1</v>
-      </c>
-      <c r="V180">
+      <c r="G180" s="7">
+        <v>44376</v>
+      </c>
+      <c r="H180" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I180" s="3">
+        <v>44377</v>
+      </c>
+      <c r="J180" s="9">
+        <v>2</v>
+      </c>
+      <c r="K180" s="2">
+        <v>1</v>
+      </c>
+      <c r="L180" s="2">
+        <v>1</v>
+      </c>
+      <c r="M180" s="2">
+        <v>1</v>
+      </c>
+      <c r="N180" s="2">
+        <v>1</v>
+      </c>
+      <c r="O180" s="2">
+        <v>1</v>
+      </c>
+      <c r="P180" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q180" s="2"/>
+      <c r="R180" s="2"/>
+      <c r="S180" s="2"/>
+      <c r="T180" s="2"/>
+      <c r="U180" s="2">
+        <v>1</v>
+      </c>
+      <c r="V180" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="181" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A181" s="2" t="s">
+      <c r="A181" t="s">
         <v>27</v>
       </c>
-      <c r="B181" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C181" s="2">
+      <c r="B181" t="s">
+        <v>30</v>
+      </c>
+      <c r="C181">
+        <f t="shared" ref="C181:C188" si="1">C180+1</f>
         <v>180</v>
       </c>
-      <c r="D181" s="7">
-        <v>43404</v>
-      </c>
-      <c r="E181" s="3" t="s">
+      <c r="D181" s="6">
+        <v>43402</v>
+      </c>
+      <c r="E181" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F181" s="8">
+      <c r="F181" s="1">
         <v>43405</v>
       </c>
-      <c r="G181" s="7">
-        <v>44376</v>
-      </c>
-      <c r="H181" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I181" s="3">
-        <v>44377</v>
-      </c>
-      <c r="J181" s="9">
-        <v>2</v>
-      </c>
-      <c r="K181" s="2">
-        <v>1</v>
-      </c>
-      <c r="L181" s="2">
-        <v>1</v>
-      </c>
-      <c r="M181" s="2">
-        <v>1</v>
-      </c>
-      <c r="N181" s="2">
-        <v>1</v>
-      </c>
-      <c r="O181" s="2">
-        <v>1</v>
-      </c>
-      <c r="P181" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q181" s="2"/>
-      <c r="R181" s="2"/>
-      <c r="S181" s="2"/>
-      <c r="T181" s="2"/>
-      <c r="U181" s="2">
-        <v>1</v>
-      </c>
-      <c r="V181" s="2">
-        <v>1</v>
+      <c r="G181" s="6">
+        <v>43420</v>
+      </c>
+      <c r="H181" t="s">
+        <v>67</v>
+      </c>
+      <c r="I181" s="1">
+        <v>43419</v>
+      </c>
+      <c r="J181" s="5"/>
+      <c r="U181">
+        <v>0.5</v>
       </c>
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.3">
@@ -17269,6 +17320,7 @@
         <v>30</v>
       </c>
       <c r="C182">
+        <f t="shared" si="1"/>
         <v>181</v>
       </c>
       <c r="D182" s="6">
@@ -17281,17 +17333,17 @@
         <v>43405</v>
       </c>
       <c r="G182" s="6">
-        <v>43420</v>
+        <v>43432</v>
       </c>
       <c r="H182" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="I182" s="1">
-        <v>43419</v>
+        <v>43434</v>
       </c>
       <c r="J182" s="5"/>
       <c r="U182">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.3">
@@ -17302,6 +17354,7 @@
         <v>30</v>
       </c>
       <c r="C183">
+        <f t="shared" si="1"/>
         <v>182</v>
       </c>
       <c r="D183" s="6">
@@ -17314,16 +17367,31 @@
         <v>43405</v>
       </c>
       <c r="G183" s="6">
-        <v>43432</v>
+        <v>43581</v>
       </c>
       <c r="H183" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I183" s="1">
-        <v>43434</v>
+        <v>43585</v>
       </c>
       <c r="J183" s="5"/>
+      <c r="K183">
+        <v>1</v>
+      </c>
+      <c r="L183">
+        <v>1</v>
+      </c>
+      <c r="M183">
+        <v>1</v>
+      </c>
+      <c r="N183">
+        <v>1</v>
+      </c>
       <c r="U183">
+        <v>1</v>
+      </c>
+      <c r="V183">
         <v>1</v>
       </c>
     </row>
@@ -17335,6 +17403,7 @@
         <v>30</v>
       </c>
       <c r="C184">
+        <f t="shared" si="1"/>
         <v>183</v>
       </c>
       <c r="D184" s="6">
@@ -17347,13 +17416,13 @@
         <v>43405</v>
       </c>
       <c r="G184" s="6">
-        <v>43581</v>
+        <v>43601</v>
       </c>
       <c r="H184" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="I184" s="1">
-        <v>43585</v>
+        <v>43600</v>
       </c>
       <c r="J184" s="5"/>
       <c r="K184">
@@ -17367,6 +17436,9 @@
       </c>
       <c r="N184">
         <v>1</v>
+      </c>
+      <c r="O184">
+        <v>0.5</v>
       </c>
       <c r="U184">
         <v>1</v>
@@ -17383,6 +17455,7 @@
         <v>30</v>
       </c>
       <c r="C185">
+        <f t="shared" si="1"/>
         <v>184</v>
       </c>
       <c r="D185" s="6">
@@ -17395,13 +17468,13 @@
         <v>43405</v>
       </c>
       <c r="G185" s="6">
-        <v>43601</v>
+        <v>43614</v>
       </c>
       <c r="H185" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="I185" s="1">
-        <v>43600</v>
+        <v>43616</v>
       </c>
       <c r="J185" s="5"/>
       <c r="K185">
@@ -17417,7 +17490,7 @@
         <v>1</v>
       </c>
       <c r="O185">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="U185">
         <v>1</v>
@@ -17434,6 +17507,7 @@
         <v>30</v>
       </c>
       <c r="C186">
+        <f t="shared" si="1"/>
         <v>185</v>
       </c>
       <c r="D186" s="6">
@@ -17446,13 +17520,13 @@
         <v>43405</v>
       </c>
       <c r="G186" s="6">
-        <v>43614</v>
+        <v>43648</v>
       </c>
       <c r="H186" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I186" s="1">
-        <v>43616</v>
+        <v>43646</v>
       </c>
       <c r="J186" s="5"/>
       <c r="K186">
@@ -17468,6 +17542,9 @@
         <v>1</v>
       </c>
       <c r="O186">
+        <v>1</v>
+      </c>
+      <c r="P186">
         <v>1</v>
       </c>
       <c r="U186">
@@ -17485,6 +17562,7 @@
         <v>30</v>
       </c>
       <c r="C187">
+        <f t="shared" si="1"/>
         <v>186</v>
       </c>
       <c r="D187" s="6">
@@ -17497,13 +17575,13 @@
         <v>43405</v>
       </c>
       <c r="G187" s="6">
-        <v>43648</v>
+        <v>43683</v>
       </c>
       <c r="H187" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I187" s="1">
-        <v>43646</v>
+        <v>43677</v>
       </c>
       <c r="J187" s="5"/>
       <c r="K187">
@@ -17524,6 +17602,9 @@
       <c r="P187">
         <v>1</v>
       </c>
+      <c r="Q187">
+        <v>1</v>
+      </c>
       <c r="U187">
         <v>1</v>
       </c>
@@ -17532,119 +17613,63 @@
       </c>
     </row>
     <row r="188" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A188" t="s">
+      <c r="A188" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B188" t="s">
+      <c r="B188" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C188">
+      <c r="C188" s="13">
+        <f t="shared" si="1"/>
         <v>187</v>
       </c>
-      <c r="D188" s="6">
+      <c r="D188" s="7">
         <v>43402</v>
       </c>
-      <c r="E188" s="1" t="s">
+      <c r="E188" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F188" s="1">
+      <c r="F188" s="8">
         <v>43405</v>
       </c>
-      <c r="G188" s="6">
-        <v>43683</v>
-      </c>
-      <c r="H188" t="s">
-        <v>37</v>
-      </c>
-      <c r="I188" s="1">
-        <v>43677</v>
-      </c>
-      <c r="J188" s="5"/>
-      <c r="K188">
-        <v>1</v>
-      </c>
-      <c r="L188">
-        <v>1</v>
-      </c>
-      <c r="M188">
-        <v>1</v>
-      </c>
-      <c r="N188">
-        <v>1</v>
-      </c>
-      <c r="O188">
-        <v>1</v>
-      </c>
-      <c r="P188">
-        <v>1</v>
-      </c>
-      <c r="Q188">
-        <v>1</v>
-      </c>
-      <c r="U188">
-        <v>1</v>
-      </c>
-      <c r="V188">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A189" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B189" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C189" s="2">
-        <v>188</v>
-      </c>
-      <c r="D189" s="7">
-        <v>43402</v>
-      </c>
-      <c r="E189" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F189" s="8">
-        <v>43405</v>
-      </c>
-      <c r="G189" s="7">
+      <c r="G188" s="7">
         <v>44376</v>
       </c>
-      <c r="H189" s="2" t="s">
+      <c r="H188" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I189" s="3">
+      <c r="I188" s="3">
         <v>44377</v>
       </c>
-      <c r="J189" s="9">
+      <c r="J188" s="9">
         <v>2</v>
       </c>
-      <c r="K189" s="2">
-        <v>1</v>
-      </c>
-      <c r="L189" s="2">
-        <v>1</v>
-      </c>
-      <c r="M189" s="2">
-        <v>1</v>
-      </c>
-      <c r="N189" s="2">
-        <v>1</v>
-      </c>
-      <c r="O189" s="2">
-        <v>1</v>
-      </c>
-      <c r="P189" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q189" s="2"/>
-      <c r="R189" s="2"/>
-      <c r="S189" s="2"/>
-      <c r="T189" s="2"/>
-      <c r="U189" s="2">
-        <v>1</v>
-      </c>
-      <c r="V189" s="2">
+      <c r="K188" s="2">
+        <v>1</v>
+      </c>
+      <c r="L188" s="2">
+        <v>1</v>
+      </c>
+      <c r="M188" s="2">
+        <v>1</v>
+      </c>
+      <c r="N188" s="2">
+        <v>1</v>
+      </c>
+      <c r="O188" s="2">
+        <v>1</v>
+      </c>
+      <c r="P188" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q188" s="2"/>
+      <c r="R188" s="2"/>
+      <c r="S188" s="2"/>
+      <c r="T188" s="2"/>
+      <c r="U188" s="2">
+        <v>1</v>
+      </c>
+      <c r="V188" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>